<commit_message>
Adjusted the size letter on the interface and the mail
</commit_message>
<xml_diff>
--- a/Logs/interaction_log.xlsx
+++ b/Logs/interaction_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="135">
   <si>
     <t>timestamp</t>
   </si>
@@ -112,6 +112,18 @@
     <t>2025-11-01T19:12:27.309548</t>
   </si>
   <si>
+    <t>2025-11-01T19:40:57.078539</t>
+  </si>
+  <si>
+    <t>2025-11-01T19:42:29.787602</t>
+  </si>
+  <si>
+    <t>2025-11-02T08:34:07.104270</t>
+  </si>
+  <si>
+    <t>2025-11-02T09:05:47.331477</t>
+  </si>
+  <si>
     <t>What are the decisions from desicion register?</t>
   </si>
   <si>
@@ -154,6 +166,9 @@
     <t>What was management's response to the System Council's feedback on the governance of breeding programs and genebanks?</t>
   </si>
   <si>
+    <t>What were the System Council's decisions regarding appointments to the Intellectual Property Group?</t>
+  </si>
+  <si>
     <t>You are a helpful assistant that answer user questions in a detailed and comprehensive way.</t>
   </si>
   <si>
@@ -197,6 +212,9 @@
   </si>
   <si>
     <t>pdf:SC22-Resource_SC-Action-Tracker.pdf:p2pt1:0.779, pdf:SC21-16_Meeting Summary_Approved.pdf:p46pt2:0.688, xlsx:CGIAR System Council Decisions.xlsx:row68:0.666, pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p14pt4:0.644, pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p14pt1:0.644, xlsx:CGIAR System Council Decisions.xlsx:row202:0.641, pdf:SC17-16_MeetingSummary_Approved_.pdf:p11pt1:0.636, pdf:SC21-16_Meeting Summary_Approved.pdf:p47pt1:0.632, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p32pt4:0.625, pdf:SC21-16_Meeting Summary_Approved.pdf:p22pt4:0.622, pdf:SC19-23_MeetingSummary-Approved.pdf:p17pt1:0.621, pdf:SC21-16_Meeting Summary_Approved.pdf:p21pt4:0.621, pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p14pt2:0.619, pdf:SC17-16_MeetingSummary_Approved_.pdf:p24pt4:0.613, pdf:SC21_Chair's Summary.pdf:p5pt3:0.609, pdf:SC19-23_MeetingSummary-Approved.pdf:p11pt1:0.604, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p9pt1:0.601, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p8pt4:0.598, pdf:SC21-16_Meeting Summary_Approved.pdf:p46pt3:0.597, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p7pt1:0.596, pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p13pt2:0.594, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p6pt4:0.593, pdf:SC16-ChairSummary_July2022.pdf:p4pt2:0.592, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p48pt2:0.590, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p49pt1:0.589, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p49pt2:0.588, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p17pt4:0.588, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p55pt1:0.587, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p12pt2:0.584, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p12pt2:0.584, pdf:SC20-19_Meeting Summary_APPROVED.pdf:p42pt4:0.584, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p49pt4:0.580, pdf:SC22-20_Meeting Summary_Approved.pdf:p13pt1:0.578, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p6pt2:0.577, pdf:INIT05-Market-Intelligence-and-Product-Profiling.pdf:p29pt4:0.576, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p52pt2:0.574, pdf:SC21-16_Meeting Summary_Approved.pdf:p22pt1:0.572, pdf:SC19-23_MeetingSummary-Approved.pdf:p11pt2:0.571, pdf:INIT01-Accelerated-Breeding-ABI-Meeting-Farmers-Needs-with-Nutritious-Climate-Resilient-Crops.pdf:p45pt2:0.568, pdf:SC19-23_MeetingSummary-Approved.pdf:p17pt2:0.567, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p53pt1:0.565, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p23pt4:0.564, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p23pt4:0.564, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p25pt2:0.563, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p14pt3:0.563, pdf:SC16-ChairSummary_July2022.pdf:p2pt2:0.562, xlsx:CGIAR System Council Decisions.xlsx:row118:0.562, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p9pt2:0.562, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p37pt1:0.561, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p34pt4:0.559, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p34pt4:0.559, pdf:SC18-17_MeetingSummary_APPROVED.pdf:p35pt2:0.559, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p52pt3:0.557, pdf:SC22-20_Meeting Summary_Approved.pdf:p41pt4:0.556, pdf:SC19-23_MeetingSummary-Approved.pdf:p16pt4:0.555, pdf:INIT01-Accelerated-Breeding-ABI-Meeting-Farmers-Needs-with-Nutritious-Climate-Resilient-Crops.pdf:p24pt1:0.555, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p6pt3:0.555, pdf:Item 4 Presentation - Update on the Inception Phase for the 2025--30 Portfolio, June 2025.pdf:p23pt1:0.554, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p36pt3:0.553, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p36pt3:0.553, pdf:SC17-16_MeetingSummary_Approved_.pdf:p11pt4:0.553, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p47pt1:0.552, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p59pt3:0.551, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p59pt3:0.551, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p20pt1:0.551, pdf:GEdI-Final-Proposal-May-12-FINAL.pdf:p53pt1:0.551, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p13pt4:0.550, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p34pt3:0.549, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p34pt3:0.549, pdf:INIT17-Sustainable-Animal-Productivity-for Livelihoods-Nutrition-and-Gender-inclusion SAPLING.pdf:p7pt4:0.549, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p23pt1:0.549, pdf:SC21-16_Meeting Summary_Approved.pdf:p31pt4:0.548, pdf:SC19-23_MeetingSummary-Approved.pdf:p17pt3:0.548, pdf:INIT01-Accelerated-Breeding-ABI-Meeting-Farmers-Needs-with-Nutritious-Climate-Resilient-Crops.pdf:p24pt3:0.548, pdf:Item 4 Presentation - Update on the Inception Phase for the 2025--30 Portfolio, June 2025.pdf:p24pt1:0.548, pdf:SC19_Chairs-Summary_Final_27Oct2023.pdf:p8pt4:0.547, pdf:SC21-16_Meeting Summary_Approved.pdf:p50pt1:0.547, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p6pt1:0.546, pdf:INIT05-Market-Intelligence-and-Product-Profiling.pdf:p30pt4:0.545, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p36pt2:0.545, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p39pt1:0.544, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p35pt4:0.544, pdf:INIT01-Accelerated-Breeding-ABI-Meeting-Farmers-Needs-with-Nutritious-Climate-Resilient-Crops.pdf:p25pt3:0.544, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p1pt1:0.543, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p35pt3:0.542, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p29pt2:0.540, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p12pt3:0.539, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p12pt3:0.539, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p28pt4:0.539, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p28pt4:0.539, pdf:SC22_Chair's Summary_Final.pdf:p9pt2:0.538, pdf:INIT01-Accelerated-Breeding-ABI-Meeting-Farmers-Needs-with-Nutritious-Climate-Resilient-Crops.pdf:p10pt1:0.537, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p11pt4:0.537, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p11pt4:0.537, pdf:SC16-ChairSummary_July2022.pdf:p5pt4:0.537, pdf:INIT06-Delivering-Genetic-Gains-in-Farmers-Fields-SeEdQUAL.pdf:p17pt2:0.535, pdf:SC21-16_Meeting Summary_Approved.pdf:p31pt3:0.535, pdf:SC20_Chairs-Summary.pdf:p2pt2:0.535, pdf:INIT34-Livestock-Climate-and-System-Resilience-LCSR.pdf:p9pt1:0.535, pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p13pt3:0.534, pdf:INIT06-Delivering-Genetic-Gains-in-Farmers-Fields-SeEdQUAL.pdf:p34pt1:0.533, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p8pt2:0.533, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p8pt2:0.533, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p42pt2:0.532, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p42pt2:0.532, pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p15pt4:0.532, pdf:GEdI-Final-Proposal-May-12-FINAL.pdf:p46pt4:0.531, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p54pt3:0.530, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p54pt3:0.530, pdf:INIT34-Livestock-Climate-and-System-Resilience-LCSR.pdf:p51pt1:0.530, pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p12pt4:0.530, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p56pt2:0.529, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p56pt2:0.529, pdf:SC18-17_MeetingSummary_APPROVED.pdf:p20pt2:0.529, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p10pt1:0.529, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p20pt2:0.528, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p27pt1:0.527, pdf:SC19-23_MeetingSummary-Approved.pdf:p15pt4:0.527, xlsx:CGIAR System Council Decisions.xlsx:row261:0.527, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p56pt3:0.526, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p56pt3:0.526, pdf:INIT06-Delivering-Genetic-Gains-in-Farmers-Fields-SeEdQUAL.pdf:p9pt1:0.526, pdf:SC18-17_MeetingSummary_APPROVED.pdf:p25pt3:0.525, pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p6pt1:0.524, pdf:INIT05-Market-Intelligence-and-Product-Profiling.pdf:p21pt2:0.524, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p45pt1:0.524, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p36pt4:0.524, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p43pt1:0.524, pdf:INIT07-Protecting-Human-Health-through-a-One-Health-Approach-PDF.pdf:p44pt4:0.524, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p46pt3:0.524, pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p15pt3:0.524, pdf:Companion-Document-to-2022-2024-CGIAR-Investment-Prospectus.pdf:p7pt2:0.523, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p48pt3:0.523, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p48pt3:0.523, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p16pt4:0.522, pdf:INIT17-Sustainable-Animal-Productivity-for Livelihoods-Nutrition-and-Gender-inclusion SAPLING.pdf:p60pt1:0.522, pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p13pt4:0.521, pdf:INIT06-Delivering-Genetic-Gains-in-Farmers-Fields-SeEdQUAL.pdf:p65pt1:0.520, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p47pt4:0.520, pdf:SC20_Chairs-Summary.pdf:p2pt3:0.520, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p15pt1:0.520, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p48pt1:0.519, pdf:Item 4 Presentation - Update on the Inception Phase for the 2025--30 Portfolio, June 2025.pdf:p3pt4:0.519, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p25pt1:0.519, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p38pt2:0.518, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p40pt1:0.518, pdf:SC18-17_MeetingSummary_APPROVED.pdf:p25pt2:0.517, pdf:INIT06-Delivering-Genetic-Gains-in-Farmers-Fields-SeEdQUAL.pdf:p54pt1:0.517, pdf:INIT21-Ukama-Ustawi-Diversification-for-resilient-agribusiness-ecosystems-in-East-and-Southern-Africa-ESA-.pdf:p57pt2:0.517, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p13pt1:0.517, pdf:INIT05-Market-Intelligence-and-Product-Profiling.pdf:p18pt4:0.517, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p1pt3:0.516, pdf:INIT06-Delivering-Genetic-Gains-in-Farmers-Fields-SeEdQUAL.pdf:p4pt3:0.516, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p18pt3:0.515, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p18pt3:0.515, pdf:INIT17-Sustainable-Animal-Productivity-for Livelihoods-Nutrition-and-Gender-inclusion SAPLING.pdf:p9pt2:0.515, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p46pt2:0.515, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p8pt2:0.514, pdf:GEdI-Final-Proposal-May-12-FINAL.pdf:p10pt3:0.513, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p57pt1:0.513, pdf:Target-funding-for-the-CGIAR-portfolio-for-the-2022-24-business-cycle.pdf:p3pt4:0.512, pdf:INIT06-Delivering-Genetic-Gains-in-Farmers-Fields-SeEdQUAL.pdf:p9pt4:0.512, pdf:F2R-CWANA.pdf:p5pt4:0.512, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p11pt3:0.512, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p11pt3:0.512, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p14pt1:0.512, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p5pt3:0.512, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p42pt4:0.511, pdf:INIT01-Accelerated-Breeding-ABI-Meeting-Farmers-Needs-with-Nutritious-Climate-Resilient-Crops.pdf:p11pt1:0.511, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p1pt2:0.511, pdf:TAFS_WCA.pdf:p56pt1:0.510, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p4pt1:0.510, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p31pt3:0.510, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p31pt3:0.510, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p50pt1:0.510, pdf:F2R-CWANA.pdf:p19pt4:0.510, pdf:INIT01-Accelerated-Breeding-ABI-Meeting-Farmers-Needs-with-Nutritious-Climate-Resilient-Crops.pdf:p8pt1:0.510, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p8pt1:0.509, pdf:SC19-23_MeetingSummary-Approved.pdf:p44pt1:0.509, pdf:INIT01-Accelerated-Breeding-ABI-Meeting-Farmers-Needs-with-Nutritious-Climate-Resilient-Crops.pdf:p43pt4:0.509, pdf:INIT05-Market-Intelligence-and-Product-Profiling.pdf:p30pt3:0.509, pdf:INIT05-Market-Intelligence-and-Product-Profiling.pdf:p8pt3:0.509, pdf:INIT05-Market-Intelligence-and-Product-Profiling.pdf:p43pt2:0.509, pdf:F2R-CWANA.pdf:p54pt1:0.508, pdf:Item 4 Presentation - Update on the Inception Phase for the 2025--30 Portfolio, June 2025.pdf:p24pt2:0.508, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p53pt2:0.508, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p7pt2:0.508, pdf:SC19-23_MeetingSummary-Approved.pdf:p34pt4:0.508, pdf:INIT01-Accelerated-Breeding-ABI-Meeting-Farmers-Needs-with-Nutritious-Climate-Resilient-Crops.pdf:p45pt3:0.507, pdf:INIT06-Delivering-Genetic-Gains-in-Farmers-Fields-SeEdQUAL.pdf:p34pt3:0.507, pdf:F2R-CWANA.pdf:p52pt1:0.507, pdf:SC18-17_MeetingSummary_APPROVED.pdf:p6pt1:0.507, pdf:HER.pdf:p36pt4:0.507, pdf:INIT06-Delivering-Genetic-Gains-in-Farmers-Fields-SeEdQUAL.pdf:p53pt1:0.507, pdf:GEdI-Final-Proposal-May-12-FINAL.pdf:p57pt4:0.506, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p56pt2:0.506, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p32pt4:0.505, pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p32pt4:0.505, pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p51pt1:0.505, pdf:INIT06-Delivering-Genetic-Gains-in-Farmers-Fields-SeEdQUAL.pdf:p28pt4:0.505</t>
+  </si>
+  <si>
+    <t>xlsx:CGIAR System Council Decisions.xlsx:row183:0.760, xlsx:CGIAR System Council Decisions.xlsx:row96:0.751, xlsx:CGIAR System Council Decisions.xlsx:row226:0.734, xlsx:CGIAR System Council Decisions.xlsx:row208:0.723, xlsx:CGIAR System Council Decisions.xlsx:row232:0.717, xlsx:CGIAR System Council Decisions.xlsx:row94:0.715, xlsx:CGIAR System Council Decisions.xlsx:row85:0.695, xlsx:CGIAR System Council Decisions.xlsx:row1:0.671, xlsx:CGIAR System Council Decisions.xlsx:row131:0.665, xlsx:CGIAR System Council Decisions.xlsx:row265:0.646, xlsx:CGIAR System Council Decisions.xlsx:row292:0.607, xlsx:CGIAR System Council Decisions.xlsx:row67:0.602, xlsx:CGIAR System Council Decisions.xlsx:row278:0.602, xlsx:CGIAR System Council Decisions.xlsx:row119:0.599, pdf:SC22-14_AOC Report to SC22.pdf:p3pt3:0.596, xlsx:CGIAR System Council Decisions.xlsx:row293:0.592, xlsx:CGIAR System Council Decisions.xlsx:row281:0.589, xlsx:CGIAR System Council Decisions.xlsx:row50:0.588, xlsx:CGIAR System Council Decisions.xlsx:row129:0.587, xlsx:CGIAR System Council Decisions.xlsx:row49:0.586, xlsx:CGIAR System Council Decisions.xlsx:row78:0.583, pdf:SC22-08 - Governance Updates.pdf:p3pt1:0.583, xlsx:CGIAR System Council Decisions.xlsx:row17:0.579, xlsx:CGIAR System Council Decisions.xlsx:row146:0.578, xlsx:CGIAR System Council Decisions.xlsx:row223:0.576, xlsx:CGIAR System Council Decisions.xlsx:row143:0.575, pdf:SC22-20_Meeting Summary_Approved.pdf:p34pt3:0.573, pdf:SC17-16_MeetingSummary_Approved_.pdf:p22pt4:0.572, xlsx:CGIAR System Council Decisions.xlsx:row205:0.566, xlsx:CGIAR System Council Decisions.xlsx:row31:0.565, xlsx:CGIAR System Council Decisions.xlsx:row88:0.564, xlsx:CGIAR System Council Decisions.xlsx:row184:0.564, xlsx:CGIAR System Council Decisions.xlsx:row148:0.563, pdf:SC18-17_MeetingSummary_APPROVED.pdf:p2pt1:0.563, xlsx:CGIAR System Council Decisions.xlsx:row162:0.563, xlsx:CGIAR System Council Decisions.xlsx:row74:0.563, xlsx:CGIAR System Council Decisions.xlsx:row51:0.561, xlsx:CGIAR System Council Decisions.xlsx:row106:0.561, pdf:SC22-Resource_SC-Action-Tracker.pdf:p1pt2:0.561, xlsx:CGIAR System Council Decisions.xlsx:row189:0.560, xlsx:CGIAR System Council Decisions.xlsx:row60:0.559, pdf:SC20_Chairs-Summary.pdf:p5pt1:0.559, xlsx:CGIAR System Council Decisions.xlsx:row30:0.556, xlsx:CGIAR System Council Decisions.xlsx:row251:0.556, xlsx:CGIAR System Council Decisions.xlsx:row230:0.555, xlsx:CGIAR System Council Decisions.xlsx:row195:0.555, pdf:SC17-16_MeetingSummary_Approved_.pdf:p23pt1:0.554, xlsx:CGIAR System Council Decisions.xlsx:row97:0.554, pdf:SC17-16_MeetingSummary_Approved_.pdf:p1pt2:0.554, pdf:SC17-16_MeetingSummary_Approved_.pdf:p23pt2:0.554, xlsx:CGIAR System Council Decisions.xlsx:row225:0.553, pdf:SC18-17_MeetingSummary_APPROVED.pdf:p10pt1:0.552, pdf:SC22-Resource_SC-Action-Tracker.pdf:p1pt1:0.552, xlsx:CGIAR System Council Decisions.xlsx:row92:0.552, xlsx:CGIAR System Council Decisions.xlsx:row63:0.551, pdf:SC22-14_AOC Report to SC22.pdf:p3pt2:0.549, xlsx:CGIAR System Council Decisions.xlsx:row53:0.549, xlsx:CGIAR System Council Decisions.xlsx:row40:0.549, xlsx:CGIAR System Council Decisions.xlsx:row47:0.549, pdf:SC-adhoc-20December2023_MeetingSummary-APPROVED.pdf:p3pt2:0.549, xlsx:CGIAR System Council Decisions.xlsx:row98:0.549, xlsx:CGIAR System Council Decisions.xlsx:row255:0.547, xlsx:CGIAR System Council Decisions.xlsx:row37:0.547, xlsx:CGIAR System Council Decisions.xlsx:row137:0.547, pdf:SC-adhoc-20December2023_MeetingSummary-APPROVED.pdf:p1pt2:0.546, pdf:SC18-17_MeetingSummary_APPROVED.pdf:p21pt1:0.546, xlsx:CGIAR System Council Decisions.xlsx:row32:0.546, xlsx:CGIAR System Council Decisions.xlsx:row52:0.546, pdf:SC20_Chairs-Summary.pdf:p2pt3:0.544, pdf:SC22-14_AOC Report to SC22.pdf:p1pt2:0.544, pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p2pt2:0.544, pdf:SC21-16_Meeting Summary_Approved.pdf:p47pt1:0.543, pdf:SC21-16_Meeting Summary_Approved.pdf:p22pt4:0.542, xlsx:CGIAR System Council Decisions.xlsx:row132:0.541, xlsx:CGIAR System Council Decisions.xlsx:row160:0.539, xlsx:CGIAR System Council Decisions.xlsx:row161:0.536, pdf:SC18_Chairs_Summary_Issued_25May2023.pdf:p4pt1:0.534, xlsx:CGIAR System Council Decisions.xlsx:row76:0.534, pdf:SC21-16_Meeting Summary_Approved.pdf:p26pt1:0.534, pdf:SC21-16_Meeting Summary_Approved.pdf:p37pt2:0.534, pdf:SC22_Chair's Summary_Final.pdf:p6pt2:0.533, xlsx:CGIAR System Council Decisions.xlsx:row140:0.533, pdf:SC21-16_Meeting Summary_Approved.pdf:p35pt2:0.532, xlsx:CGIAR System Council Decisions.xlsx:row236:0.532, pdf:SC22-20_Meeting Summary_Approved.pdf:p24pt4:0.532, pdf:SC18_Chairs_Summary_Issued_25May2023.pdf:p6pt2:0.531, pdf:SC22-15 NCSC Report 5 to the System Council.pdf:p1pt2:0.531, xlsx:CGIAR System Council Decisions.xlsx:row141:0.531, xlsx:CGIAR System Council Decisions.xlsx:row156:0.531, xlsx:CGIAR System Council Decisions.xlsx:row54:0.531, xlsx:CGIAR System Council Decisions.xlsx:row111:0.531, pdf:SC-adhoc-20December2023_MeetingSummary-APPROVED.pdf:p2pt1:0.530, pdf:SC22-14_AOC Report to SC22.pdf:p7pt4:0.530, pdf:SC22-20_Meeting Summary_Approved.pdf:p37pt2:0.530, pdf:SC22-06a - Incentives WG - Inception Report with Annexes.pdf:p17pt4:0.529, xlsx:CGIAR System Council Decisions.xlsx:row257:0.529, pdf:SC22-10b SPIA Nomination for new Panel Member.pdf:p1pt3:0.528, pdf:SC17-16_MeetingSummary_Approved_.pdf:p1pt4:0.528, pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p1pt2:0.528, xlsx:CGIAR System Council Decisions.xlsx:row130:0.527, pdf:SC21-16_Meeting Summary_Approved.pdf:p46pt2:0.526, pdf:Item 15 Presentation - NCSC Report to SC22.pdf:p1pt3:0.526, xlsx:CGIAR System Council Decisions.xlsx:row21:0.526, xlsx:CGIAR System Council Decisions.xlsx:row260:0.525, pdf:SC21-16_Meeting Summary_Approved.pdf:p28pt4:0.524, pdf:SC21_Chair's Summary.pdf:p5pt2:0.524, xlsx:CGIAR System Council Decisions.xlsx:row170:0.523, xlsx:CGIAR System Council Decisions.xlsx:row234:0.523, pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p12pt1:0.523, xlsx:CGIAR System Council Decisions.xlsx:row224:0.523, xlsx:CGIAR System Council Decisions.xlsx:row48:0.522, pdf:SC18-17_MeetingSummary_APPROVED.pdf:p20pt1:0.522, pdf:SC22-20_Meeting Summary_Approved.pdf:p27pt2:0.522, xlsx:CGIAR System Council Decisions.xlsx:row279:0.520, xlsx:CGIAR System Council Decisions.xlsx:row172:0.520, pdf:SC19-23_MeetingSummary-Approved.pdf:p1pt4:0.520, pdf:SC17_Chairs_Summary_Issued_6Nov2022.pdf:p4pt4:0.520, pdf:SC22-15 NCSC Report 5 to the System Council.pdf:p1pt4:0.519, xlsx:CGIAR System Council Decisions.xlsx:row82:0.519, pdf:SC-adhoc-20December2023_MeetingSummary-APPROVED.pdf:p2pt2:0.518, pdf:SC18-17_MeetingSummary_APPROVED.pdf:p23pt4:0.517, pdf:SC22_Chair's Summary_Final.pdf:p6pt4:0.517, pdf:SC22-06a - Incentives WG - Inception Report with Annexes.pdf:p39pt4:0.517, xlsx:CGIAR System Council Decisions.xlsx:row259:0.517, pdf:SC17-16_MeetingSummary_Approved_.pdf:p4pt4:0.516, xlsx:CGIAR System Council Decisions.xlsx:row90:0.516, pdf:SC22-15 NCSC Report 5 to the System Council.pdf:p2pt2:0.514, pdf:SC22-08 - Governance Updates.pdf:p4pt3:0.514, pdf:SC22-01_Agenda-Adopted.pdf:p4pt2:0.514, pdf:SC21-16_Meeting Summary_Approved.pdf:p46pt4:0.514, xlsx:CGIAR System Council Decisions.xlsx:row66:0.514, pdf:Item 9 Presentation - SIMEC Report to SC22.pdf:p2pt1:0.513, xlsx:CGIAR System Council Decisions.xlsx:row286:0.513, xlsx:CGIAR System Council Decisions.xlsx:row56:0.513, pdf:SC19_Chairs-Summary_Final_27Oct2023.pdf:p5pt4:0.512, xlsx:CGIAR System Council Decisions.xlsx:row38:0.511, xlsx:CGIAR System Council Decisions.xlsx:row228:0.511, xlsx:CGIAR System Council Decisions.xlsx:row294:0.509, pdf:Item 15 Presentation - NCSC Report to SC22.pdf:p1pt1:0.509, pdf:SC18-17_MeetingSummary_APPROVED.pdf:p11pt1:0.507, xlsx:CGIAR System Council Decisions.xlsx:row206:0.507, pdf:SC21_Chair's Summary.pdf:p5pt3:0.506, pdf:SC17-16_MeetingSummary_Approved_.pdf:p23pt4:0.506, pdf:SC20-19_Meeting Summary_APPROVED.pdf:p22pt4:0.505, pdf:Resource_Out-of-session-decisions-since-SC21.pdf:p2pt3:0.505, xlsx:CGIAR System Council Decisions.xlsx:row61:0.504, pdf:SC21-16_Meeting Summary_Approved.pdf:p35pt1:0.504, pdf:SC22-01_Provisional-Agenda Annotated.pdf:p7pt4:0.504, pdf:SC17-16_MeetingSummary_Approved_.pdf:p29pt4:0.504, pdf:SC22-06a - Incentives WG - Inception Report with Annexes.pdf:p17pt2:0.504, pdf:SC18-17_MeetingSummary_APPROVED.pdf:p1pt2:0.504, xlsx:CGIAR System Council Decisions.xlsx:row193:0.502, pdf:SC20-19_Meeting Summary_APPROVED.pdf:p20pt4:0.502, xlsx:CGIAR System Council Decisions.xlsx:row93:0.502, xlsx:CGIAR System Council Decisions.xlsx:row18:0.501, pdf:SC18-17_MeetingSummary_APPROVED.pdf:p37pt1:0.500, pdf:SC20-19_Meeting Summary_APPROVED.pdf:p26pt1:0.500, pdf:SC17-16_MeetingSummary_Approved_.pdf:p21pt1:0.500, pdf:SC20-19_Meeting Summary_APPROVED.pdf:p5pt4:0.500, pdf:SC17-16_MeetingSummary_Approved_.pdf:p29pt1:0.500, pdf:SC20-19_Meeting Summary_APPROVED.pdf:p24pt2:0.499, pdf:SC22-20_Meeting Summary_Approved.pdf:p35pt2:0.499, pdf:SC21-16_Meeting Summary_Approved.pdf:p2pt1:0.499, xlsx:CGIAR System Council Decisions.xlsx:row157:0.499, pdf:SC22-20_Meeting Summary_Approved.pdf:p34pt2:0.498, pdf:SC21-16_Meeting Summary_Approved.pdf:p47pt2:0.498, pdf:SC17_Chairs_Summary_Issued_6Nov2022.pdf:p4pt1:0.498, pdf:SC17-16_MeetingSummary_Approved_.pdf:p24pt3:0.498, pdf:SC22-06a - Incentives WG - Inception Report with Annexes.pdf:p20pt3:0.498, xlsx:CGIAR System Council Decisions.xlsx:row87:0.498, pdf:SC21-16_Meeting Summary_Approved.pdf:p23pt1:0.497, pdf:SC22-07a - ROP - Status Report to SC22.pdf:p1pt2:0.497, pdf:SC21_Chair's Summary.pdf:p5pt1:0.497, pdf:SC19_Chairs-Summary_Final_27Oct2023.pdf:p4pt2:0.497, pdf:Item 14 Presentation - AOC presentation to SC22.pdf:p9pt3:0.496, xlsx:CGIAR System Council Decisions.xlsx:row197:0.496, xlsx:CGIAR System Council Decisions.xlsx:row261:0.496, xlsx:CGIAR System Council Decisions.xlsx:row210:0.496, xlsx:CGIAR System Council Decisions.xlsx:row198:0.495, pdf:SC-adhoc-20December2023_MeetingSummary-APPROVED.pdf:p4pt3:0.495, xlsx:CGIAR System Council Decisions.xlsx:row75:0.495, xlsx:CGIAR System Council Decisions.xlsx:row288:0.494, pdf:SC22-20_Meeting Summary_Approved.pdf:p1pt3:0.494, pdf:SC18-17_MeetingSummary_APPROVED.pdf:p13pt1:0.494, pdf:SC22-Resource_SC-Action-Tracker.pdf:p6pt1:0.494, xlsx:CGIAR System Council Decisions.xlsx:row229:0.494, pdf:SC22-20_Meeting Summary_Approved.pdf:p25pt4:0.493, pdf:SC22-20_Meeting Summary_Approved.pdf:p35pt1:0.493, pdf:SC21-16_Meeting Summary_Approved.pdf:p5pt2:0.493, xlsx:CGIAR System Council Decisions.xlsx:row10:0.493, xlsx:CGIAR System Council Decisions.xlsx:row22:0.493, pdf:SC17_Chairs_Summary_Issued_6Nov2022.pdf:p5pt1:0.493, pdf:SC22-08 - Governance Updates.pdf:p2pt2:0.492, pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p2pt1:0.491, pdf:SC18-17_MeetingSummary_APPROVED.pdf:p20pt2:0.491, pdf:SC22-01_Agenda-Adopted.pdf:p4pt3:0.490, pdf:SC22-06a - Incentives WG - Inception Report with Annexes.pdf:p21pt2:0.490, xlsx:CGIAR System Council Decisions.xlsx:row177:0.490, pdf:SC17-16_MeetingSummary_Approved_.pdf:p32pt1:0.490, xlsx:CGIAR System Council Decisions.xlsx:row89:0.490</t>
   </si>
   <si>
     <t>The decisions from the decision register include various actions taken by the System Council during its meetings. Here are some notable decisions:
@@ -381,6 +399,50 @@
 **Used Sources:** xlsx:CGIAR System Council Decisions.xlsx:row183, xlsx:CGIAR System Council Decisions.xlsx:row96, xlsx:CGIAR System Council Decisions.xlsx:row208, xlsx:CGIAR System Council Decisions.xlsx:row232, xlsx:CGIAR System Council Decisions.xlsx:row85, xlsx:CGIAR System Council Decisions.xlsx:row1.</t>
   </si>
   <si>
+    <t>The System Council made several decisions regarding appointments to the Intellectual Property Group (IP Group) over different dates. Here are the key decisions:
+1. **Extension of Membership (March 2020)**: The System Council extended the membership of certain individuals to the Intellectual Property Group until December 31, 2021. These members serve in a personal capacity and not as representatives of any constituencies of the System Council (ID: xlsx:CGIAR System Council Decisions.xlsx:row183).
+2. **Formation of Nominations Committee (March 2023)**: The System Council approved the formation of an ad-hoc Nominations Committee to select members for the Intellectual Property Group for a two-year term. This committee includes the Chair of the Strategic Impact, Monitoring and Evaluation Committee (SIMEC), the Chair of the Assurance Oversight Committee (AOC), and an independent member with expertise in intellectual property assets management (ID: xlsx:CGIAR System Council Decisions.xlsx:row96).
+3. **Membership Extension (March 2019)**: The membership of Aline Flower and Bram De Jonge was extended until December 31, 2019, with the same stipulation that they serve in a personal capacity (ID: xlsx:CGIAR System Council Decisions.xlsx:row208).
+4. **Interim Membership Extension (September 2018)**: An interim extension of membership for Paul Figueroa, Bram De Jonge, and Aline Flower was approved until July 31, 2018, again noting that they serve in a personal capacity (ID: xlsx:CGIAR System Council Decisions.xlsx:row232).
+5. **Appointment of New Members (June 2023)**: The System Council approved the appointment of Aline Flower and Eric Huttner as members of the Intellectual Property Group for a two-year term through June 13, 2025, also noting that they serve in a personal capacity (ID: xlsx:CGIAR System Council Decisions.xlsx:row85).
+6. **Future Appointments (October 2025)**: The System Council approved the appointment of Clément Aubert, Aline Flower, and Eric Huttner to the Intellectual Property Group for a term starting on November 1, 2025 (ID: xlsx:CGIAR System Council Decisions.xlsx:row1).
+These decisions reflect the ongoing management and governance of the Intellectual Property Group within the CGIAR System Council, ensuring that the group is staffed with qualified individuals while maintaining the principle that members serve in a personal capacity.
+**Used Sources:** xlsx:CGIAR System Council Decisions.xlsx:row183, xlsx:CGIAR System Council Decisions.xlsx:row96, xlsx:CGIAR System Council Decisions.xlsx:row208, xlsx:CGIAR System Council Decisions.xlsx:row232, xlsx:CGIAR System Council Decisions.xlsx:row85, xlsx:CGIAR System Council Decisions.xlsx:row1.</t>
+  </si>
+  <si>
+    <t>The System Council made several decisions regarding appointments to the Intellectual Property Group (IP Group) over different dates. Here are the key decisions:
+1. **Extension of Membership (March 2020)**: The System Council extended the membership of certain individuals to the IP Group until December 31, 2021. These members serve in a personal capacity and not as representatives of any constituencies of the System Council (ID: xlsx:CGIAR System Council Decisions.xlsx:row183).
+2. **Formation of Nominations Committee (March 2023)**: The System Council approved the formation of an ad-hoc Nominations Committee to select members for the IP Group for a two-year term. This committee includes the Chair of the Strategic Impact, Monitoring and Evaluation Committee (SIMEC), the Chair of the Assurance Oversight Committee (AOC), and an independent member with expertise in intellectual property assets management (ID: xlsx:CGIAR System Council Decisions.xlsx:row96).
+3. **Membership Extension (March 2019)**: The membership of Aline Flower and Bram De Jonge was extended until December 31, 2019, with the same stipulation that they serve in a personal capacity (ID: xlsx:CGIAR System Council Decisions.xlsx:row208).
+4. **Interim Membership Extension (September 2018)**: An interim extension of membership for Paul Figueroa, Bram De Jonge, and Aline Flower was approved until July 31, 2018 (ID: xlsx:CGIAR System Council Decisions.xlsx:row232).
+5. **New Appointments (June 2023)**: The System Council approved the appointment of Aline Flower and Eric Huttner as members of the IP Group for a two-year term through June 13, 2025, also noting that they serve in a personal capacity (ID: xlsx:CGIAR System Council Decisions.xlsx:row85).
+6. **Future Appointments (October 2025)**: The System Council approved the appointment of Clément Aubert, Aline Flower, and Eric Huttner to the IP Group for a two-year term starting November 1, 2025 (ID: xlsx:CGIAR System Council Decisions.xlsx:row1).
+These decisions reflect the ongoing management and governance of the Intellectual Property Group within the CGIAR System Council, ensuring that the group is staffed with qualified individuals while maintaining the principle that members serve in a personal capacity.
+**Used Sources:** xlsx:CGIAR System Council Decisions.xlsx:row183, xlsx:CGIAR System Council Decisions.xlsx:row96, xlsx:CGIAR System Council Decisions.xlsx:row208, xlsx:CGIAR System Council Decisions.xlsx:row232, xlsx:CGIAR System Council Decisions.xlsx:row85, xlsx:CGIAR System Council Decisions.xlsx:row1.</t>
+  </si>
+  <si>
+    <t>The System Council made several decisions regarding appointments to the Intellectual Property Group (IP Group) over different dates. Here are the key decisions:
+1. **Extension of Membership (March 2020)**: The System Council extended the membership of certain individuals to the Intellectual Property Group until December 31, 2021. These members serve in a personal capacity and not as representatives of any constituencies of the System Council (ID: xlsx:CGIAR System Council Decisions.xlsx:row183).
+2. **Formation of Nominations Committee (March 2023)**: The System Council approved the formation of an ad-hoc Nominations Committee to select members for the Intellectual Property Group for a two-year term. This committee includes the Chair of the Strategic Impact, Monitoring and Evaluation Committee (SIMEC), the Chair of the Assurance Oversight Committee (AOC), and an independent member with expertise in intellectual property assets management (ID: xlsx:CGIAR System Council Decisions.xlsx:row96).
+3. **Membership Extension (March 2019)**: The membership of Aline Flower and Bram De Jonge was extended until December 31, 2019, with the same stipulation that they serve in a personal capacity (ID: xlsx:CGIAR System Council Decisions.xlsx:row208).
+4. **Interim Membership Extension (September 2018)**: An interim extension of membership for Paul Figueroa, Bram De Jonge, and Aline Flower was approved until July 31, 2018 (ID: xlsx:CGIAR System Council Decisions.xlsx:row232).
+5. **Appointment of New Members (June 2023)**: The System Council appointed Aline Flower and Eric Huttner as members of the Intellectual Property Group for a two-year term through June 13, 2025, also noting that they serve in a personal capacity (ID: xlsx:CGIAR System Council Decisions.xlsx:row85).
+6. **Future Appointments (October 2025)**: The System Council approved the appointment of Clément Aubert, Aline Flower, and Eric Huttner to the Intellectual Property Group for a two-year term starting November 1, 2025 (ID: xlsx:CGIAR System Council Decisions.xlsx:row1).
+These decisions reflect the ongoing efforts of the System Council to manage and appoint members to the Intellectual Property Group, ensuring that the group is composed of qualified individuals serving in their personal capacities.
+**Used Sources:** xlsx:CGIAR System Council Decisions.xlsx:row183, xlsx:CGIAR System Council Decisions.xlsx:row96, xlsx:CGIAR System Council Decisions.xlsx:row208, xlsx:CGIAR System Council Decisions.xlsx:row232, xlsx:CGIAR System Council Decisions.xlsx:row85, xlsx:CGIAR System Council Decisions.xlsx:row1.</t>
+  </si>
+  <si>
+    <t>The System Council made several decisions regarding appointments to the Intellectual Property Group (IP Group) over different dates. Here are the key decisions:
+1. **Extension of Membership (March 2020)**: The System Council extended the membership of certain individuals to the Intellectual Property Group until December 31, 2021. These members serve in a personal capacity and not as representatives of any constituencies.
+2. **Formation of Nominations Committee (March 2023)**: The System Council approved the formation of an ad-hoc Nominations Committee to select members for the Intellectual Property Group for a two-year term. This committee includes the Chair of the Strategic Impact, Monitoring and Evaluation Committee (SIMEC), the Chair of the Assurance Oversight Committee (AOC), and an independent member with expertise in intellectual property assets management.
+3. **Membership Extension (March 2019)**: The membership of Aline Flower and Bram De Jonge was extended until December 31, 2019, with the same stipulation of serving in a personal capacity.
+4. **Interim Membership (September 2018)**: An interim measure was taken to extend the membership of Paul Figueroa, Bram De Jonge, and Aline Flower until July 31, 2018.
+5. **New Appointments (June 2023)**: The System Council approved the appointment of Aline Flower and Eric Huttner as members of the Intellectual Property Group for a two-year term through June 13, 2025.
+6. **Future Appointments (October 2025)**: The System Council approved the appointment of Clément Aubert, Aline Flower, and Eric Huttner to the Intellectual Property Group for a term starting on November 1, 2025.
+These decisions reflect the ongoing efforts of the System Council to ensure that the Intellectual Property Group is staffed with qualified individuals who can contribute effectively to its objectives.
+**Used Sources:** xlsx:CGIAR System Council Decisions.xlsx:row183, xlsx:CGIAR System Council Decisions.xlsx:row96, xlsx:CGIAR System Council Decisions.xlsx:row208, xlsx:CGIAR System Council Decisions.xlsx:row232, xlsx:CGIAR System Council Decisions.xlsx:row85, xlsx:CGIAR System Council Decisions.xlsx:row1</t>
+  </si>
+  <si>
     <t>SC22-08 - Governance Updates.pdf — page 7 part 2 — pdf:SC22-08 - Governance Updates.pdf:p7pt2, SC22-01_Agenda-Adopted.pdf — page 1 part 3 — pdf:SC22-01_Agenda-Adopted.pdf:p1pt3, SC22-20_Meeting Summary_Approved.pdf — page 1 part 4 — pdf:SC22-20_Meeting Summary_Approved.pdf:p1pt4</t>
   </si>
   <si>
@@ -5083,6 +5145,320 @@
 quality management, cryopreservation and new phytosanitary diagnostic advances is required to improve the technical capability of the CGIAR genebanks and reduce the costs of conservation and distribution of germplasm. Failure to innovate will mean that genebank costs will stay the same or even increase, resulting in insufficient funds to ma intain genebank operations adequately. 3 3 9 NA Budget controls are in place to monitor spending and costs Communities of Practice (CoP) have been created to oversee the development of technical advances Audits and reviews contribute to improve ment of management procedures Continued partnership with the Crop Trust (beyond 2021) will ensure secure funding. Impact of introducing innovations at one or mo</t>
   </si>
   <si>
+    <t>[ID: xlsx:CGIAR System Council Decisions.xlsx:row183]
+Decision: The System Council extended the membership of the following persons to the System Council Intellectual Property Group with effect until 31 December 2021, noting that such persons serve in a personal capacity and not as a representative of any of the System Council’s constituencies:
+Date(s): 24 March 2020
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row96]
+Decision: The System Council approved the formation and membership of an ad-hoc Nominations Committee, as follows: 
+i) the Chair of the System Council’s Strategic Impact, Monitoring and Evaluation Committee (SIMEC), or their designate, acting as Chair of the Committee, 
+ii) the Chair of the System Council’s Assurance Oversight Committee (AOC), or their designate, and 
+iii) Alan Bennett acting as an independent member with expertise in intellectual property assets management;
+to select, for confirmation by the System Council, members of the System Council Intellectual Property Group ('SC IP Group') for a two-year term, in accordance with Section 3 of the SC IP Group’s Terms of Reference.
+Date(s): 23 March 2023
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row226]
+Decision: The System Council extends the membership of the following persons to the System Council Intellectual Property Group as an interim measure with effect until 31 December 2018, noting that such persons serve in a personal capacity and not as a representative of any of the System Council’s constituencies:
+a. Paul Figueroa, Chair (Resident Legal Officer, USAID/Guatemala)
+b. Bram De Jonge, Member (Seed Policy Advisor OXFAM/Wageningen University)
+c. Aline Flower, Member (Associate General Counsel, Global Development, Bill and Melinda Gates Foundation)
+Date(s): 24 September 2018
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row208]
+Decision: The System Council extends the membership of the following persons to the System Council Intellectual Property Group with effect until 31 December 2019, noting that such persons serve in a personal capacity and not as a representative of any of the System Council’s constituencies: 
+•Aline Flower, Member (Associate General Counsel, Global Development, Bill and Melinda Gates Foundation) nominated by Bill and Melinda Gates Foundation; and 
+•Bram De Jonge, Member (Seed Policy Advisor OXFAM/Wageningen University) nominated by EIARD.
+Date(s): 13 March 2019
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row232]
+Decision: The System Council extends the membership of the following persons to the System Council Intellectual Property Group as an interim measure with effect until 31 July 2018, noting that such persons serve in a personal capacity and not as a representative of any of the System Council’s constituencies:
+a. Paul Figueroa, Chair (Resident Legal Officer, USAID/Guatemala) nominated by USAID;
+b. Bram De Jonge, Member (Seed Policy Advisor OXFAM/Wageningen University) nominated by EIARD; and
+c. Aline Flower, Member (Associate General Counsel, Global Development, Bill and Melinda Gates Foundation) nominated by Bill and Melinda Gates Foundation.
+Date(s): 30 April 2018
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row94]
+Decision: Pursuant to paragraph 3 of Annex 1 to the CGIAR Intellectual Assets Principles, the System Council approved the Terms of Reference of the Ad-hoc Nominations Committee for membership of the System Council Intellectual Property Group.
+Date(s): 28 April 2023
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row85]
+Decision: The System Council approved the appointment of the following persons as members of the System Council Intellectual Property Group for a two-year term through 13 June 2025, noting that such persons serve in a personal capacity and not as a representative of any of the System Council’s constituencies:
+• Aline Flower (Associate General Counsel, Global Development, Bill &amp; Melinda Gates Foundation), nominated by the Bill &amp; Melinda Gates Foundation; and
+• Eric Huttner (Research Program Manager Crops, ACIAR), nominated by Australia.
+Date(s): 14 June 2023
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row1]
+Decision: Pursuant to the System Council Intellectual Property Group Terms of Reference, the System Council approved the appointment of the following persons as members of the System Council Intellectual Property Group for a two-year term, starting on 1 November 2025, noting that such persons serve in a personal capacity and not as a representative of any of the System Council’s constituencies: 
+1.	Clément Aubert (Director of Innovation and Valorization ; Institut de Recherche pour le Développement), 
+2.	Aline Flower (Deputy Director, Legal; Global Agricultural Development; Bill and Melinda Gates Foundation), and
+3.	Eric Huttner (Consultant, Chloroplast Consulting, as of September 2025, former Research Program Manager, Crops, Australian Centre for International Agricultural Research).
+Date(s): 14 October 2025
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row131]
+Decision: The System Council approved the extension of the following persons as members of the System Council Intellectual Property Group with effect until 31 October 2022, noting that such persons serve in a personal capacity and not as a representative of any of the System Council’s constituencies: 
+•	Aline Flower, Member (Associate General Counsel, Global Development, Bill and Melinda Gates Foundation) originally nominated by Bill and Melinda Gates Foundation; and 
+•	Bram De Jonge, Member (Seed Policy Advisor OXFAM/Wageningen University) originally nominated by EIARD.
+Date(s): 16 December 2021
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row265]
+Decision: The System Council ratifies as an interim measure with effect until 31 December 2017, the continuing membership of the System Council IP Group as follows, noting that such persons serve in a personal capacity and not as a representative of any of the System Council’s constituencies: 
+a. Paul Figueroa, Chair (Resident Legal Officer, USAID/Guatemala); 
+b. Bram De Jonge, Member (Seed Policy Advisor OXFAM/Wageningen University); and 
+c. Aline Flower, Member (Associate General Counsel, Global Development, Bill and Melinda Gates Foundation).
+Date(s): 17 February 2017
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row292]
+Decision: The System Council approved the Terms of Reference for the System Council Chair as set out in appendix 1 of meeting document SC1-02.
+Date(s): 12 July 2016
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row67]
+Decision: The System Council approved the Terms of Reference for the Nominations Committee of the System Council.
+Date(s): 20 March 2024
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row278]
+Decision: The System Council approved with immediate effect the rules of procedure for the System Council as set out in Appendix 1 to meeting document SC2-07.
+Date(s): 25 &amp; 26 September 2016
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row119]
+Decision: The System Council adopted the Agenda (document SC16-01).
+Date(s): 20 July 2022
+---
+[ID: pdf:SC22-14_AOC Report to SC22.pdf:p3pt3]
+items of the System Council’s Action Plan. To date, 11 of the 12 matters have been closed. For the remaining item on remuneration of governance officials, a review is being overseen by the Nominations Committee of the System Council, with results expected in mid-July 2025. The AOC notes that this will be a full year since the matter was first raised during SC20 in June 2024. 10. During the course of this work on the SC Action Plan, two further matters arose. One of these has been resolved and the other is in process. 11. The AOC submitted a report titled “System Council Action Plan and investigations: AOC conclusions and recommendations” to System Council V oting Members and Alternates on 21 March 2025, with an addendum on 14 April 2025. 12. The AOC provided an update on the System Council Action Plan to SC Voting Members and Alternates on 16 April 2025 and will provide a further update before the 22 nd System
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row293]
+Decision: The System Council adopted the meeting agenda for the 1st System Council meeting (document SC1-01).
+Date(s): 12 July 2016
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row281]
+Decision: The System Council adopted the Agenda as proposed in meeting document SC2-01.
+Date(s): 25 &amp; 26 September 2016
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row50]
+Decision: The System Council approved the Summary of the Ad Hoc Meeting of the System Council held on 24 July 2024
+Date(s): 22 August 2024
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row129]
+Decision: The System Council adopted the Agenda as issued on 7 March 2022 (document SC15-01, Revision 2).
+Date(s): 8-9 March 2022
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row49]
+Decision: The System Council appointed of Renaud Seligmann, representative of the World Bank to the System Council, as a member of the Assurance and Oversight Committee for a period of three years with effect from 12 September 2024, or until a successor is appointed.
+Date(s): 12 September 2024
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row78]
+Decision: The System Council adopted the Agenda, as re-issued on 18th October 2023 with revised timings and an additional item 13a titled ‘Reflections on Research Direction &amp; Funding’.
+Date(s): 21 October 2023
+---
+[ID: pdf:SC22-08 - Governance Updates.pdf:p3pt1]
+Framework and Charter Feedback documented for consideration in this next amendment process (summarized, non-exhaustive) 1 i. Roles of the System Council relating to IPB appointments ii. Refine roles/responsibilities relating to internal audit, external audit, ethics and risk management/internal controls to align with Risk &amp; Oversight Plan and address the AOC’s comments iii. Policy development
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row17]
+Decision: The System Council adopted the Agenda for the 22nd System Council meeting, as issued on 21 May 2025.
+Date(s): 4-5 June 2025
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row146]
+Decision: The System Council approved the extension of the terms of the following members of the System Council’s Assurance Oversight Committee until 30 June 2022, unless earlier determined by the System Council:
+• Saad Bounjoua
+• Maurice Goddard
+• Muriel Uzan
+• Daniel van Gilst
+Date(s): 10 June 2021
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row223]
+Decision: The System Council adopted the Agenda issued on 11 November 2018 (meeting document SC7-01).
+Date(s): 15-16 November 2018
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row143]
+Decision: The System Council approved the appointment of Dr. Raphael Nawrotzki, representative of Germany, on the System Council’s Strategic Impact, Monitoring and Evaluation Committee (SIMEC) for a period until 31 December 2021 or until such time as a successor is appointed.
+Date(s): 6 July 2021
+---
+[ID: pdf:SC22-20_Meeting Summary_Approved.pdf:p34pt3]
+an effective governance 113. The AOC Chair presented the Committee ’s key priorities for the remainder of 2025, which include overseeing ethics and business conduct matters, ensuring completion of the System Council Action Plan, providing input on upcoming Charter and Framework revisions, overseeing implementation of the ROP and related Council recommendations, advising on the Advisory Bodies’ business plans and budget, and supporting other Council activities as needed. 114. The AOC Chair presented two decision items for the Council, recognized the work of the Committee’s Secretary, and expressed gratitude to her fellow AOC members for their collaborative effort over the last months. Key Discussion Areas 115. Council members expressed their gratitude to the AOC for their work and dedication under short timelines. Specific points included: a. A suggestion that the terms of all System Council Committee Members be standardized to two, three-year terms, with exceptions for special
+---
+[ID: pdf:SC17-16_MeetingSummary_Approved_.pdf:p22pt4]
+for Impa ct Assessment, the System Council confirm ed the appointments of the following persons: a. Dr. Kyle Emerick as SPIA Standing Panel Member for an additional three -year term with effect from 1 January 2023 unless otherwise decided by the System Council; and b. Dr. Rachid Laajaj as a Special Initiative Member for an additional three -year term with effect from 1 January 2023 unless otherwise decided by the System Council. 82. Decision SC/M17/DP6 - SIMEC Membership Appointments Pursuant to paragraph 9 of the terms of reference of the System Council’s Strategic Impact, Monitoring &amp; Evaluation Committee (‘SIMEC’), the System Council: a. Appointed the following persons as members of SIMEC until 30 June 2023 or such time as a successor is appointed:
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row205]
+Decision: The System Council adopted the Agenda issued on 23 April 2019 (meeting document SC8-01)
+Date(s): 15-16 May 2019
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row31]
+Decision: The System Council approved amendments to the Rules of Procedure of the System Council, in the form dated 27 November 2024, pursuant to paragraph 14.4 of those Rules of Procedure.
+Date(s): 11-12 December 2024
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row88]
+Decision: The System Council appointed Sebastian Lesch (Germany) as a second representative from the System Council on the Ad-Hoc Committee on Governance to provide continuity, noting that Andrew Campbell’s term on the System Council is anticipated to conclude at end-July 2023.
+Date(s): 12 May 2023
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row184]
+Decision: The System Council appointed Wijnand van-Ijssel (System Council member, The Netherlands) and Stephen Potter (System Council member, Canada) to serve in the role of System Council Active Observers on the System Management Board pursuant to Article 7.6 of the Charter of the System Organization effective from the date of this decision for a period of one year or until such time as a successor is appointed.
+Date(s): 24 March 2020
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row148]
+Decision: The System Council adopted the Agenda issued on 26 May 2021 (document SC13-01)
+Date(s): 9 June 2021
+---
+[ID: pdf:SC18-17_MeetingSummary_APPROVED.pdf:p2pt1]
+Meeting Summary, 18th System Council Meeting 18th System Council Meeting SC18-17 11-12 May 2023, Washington, DC, USA Page 2 of 42 Introduction This document presents a summary of the 18th meeting of the System Council (“Council”) held on 11-12 May 2023 in Washington, DC ., USA. It follows the release of the SC1 8 Chair’s Summary (25 May 2023). By way
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row162]
+Decision: The System Council approved the extension of the terms of the following membership on the System Council’s standing committees:
+- Stephen Potter (Canada), on the Assurance Oversight Committee to 30 June 2021, unless earlier determined by the System Council
+- The eight current members of the Strategic Impact, Monitoring and Evaluation Committee to 31 December 2021, unless earlier determined by the System Council
+Date(s): 17 December 2020
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row74]
+Decision: The System Council adopted the Agenda, as issued on 12 December 2023.
+Date(s): 20 December 2023
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row51]
+Decision: The System Council approved the "Response from System Council to Management on the Risk and Oversight Action Plan (31 July 2024)"
+Date(s): 14 August 2024
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row106]
+Decision: Pursuant to paragraph 9 of the terms of reference of the System Council’s Strategic Impact, Monitoring &amp; Evaluation Committee (‘SIMEC’), the System Council:
+(a)   Appoints the following persons as members of SIMEC until 30 June 2023 or such time as a successor is appointed
+Nikita Eriksen-Hamel (Canada)
+Gary Jahn (USA)
+Fatma Sarsu (Türkiye)
+(b)  Retroactively extends the terms of all other members of SIMEC until 30 June 2023 or 
+        such time as a successor is appointed.
+Date(s): 3 November 2022
+---
+[ID: pdf:SC22-Resource_SC-Action-Tracker.pdf:p1pt2]
+additional resource for the System Council’s 22nd meeting sets out previously agreed action
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row189]
+Decision: The System Council adopted the Agenda issued on 8 November 2019 (document SC9-01).
+Date(s): 13-14 November 2019
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row60]
+Decision: The System Council adopted the Agenda for the 20th System Council meeting, as re-issued on 9 June 2024.
+Date(s): 13 June 2024
+---
+[ID: pdf:SC20_Chairs-Summary.pdf:p5pt1]
+Chair’s Summary, SC20 20th CGIAR System Council Meeting Chair’s Summary, SC20 12-13 June 2024, Brasília, Brazil Page 5 of 5 AGREED POSITIONS AND ACTIONS SC20-AP1 – Requests to the Nominations Committee of the System Council The System Council requested the Nominations Committee of the System Council to: • Operate in accordance with its proposed, revised timeline for decision -making on Integrated Partnership Board (IPB) membership, including: o a revised delivery date of a slate of IPB nominees of Monday 22 July 2024; and o a proposal to convene a virtual, extraordinary System Council meeting session to decide on the slate of nominees, on Wednesday, 24 July 2024; and • Proceed with the selection of an external firm to be contracted by the System Organization in line with its procurement and contracting policies to review the
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row30]
+Decision: The System Council approved amendments to the Terms of Reference of the System Council Chair, in the form dated 27 November 2024, pursuant to Article 5.5 of the CGIAR System Framework.
+Date(s): 11-12 December 2024
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row251]
+Decision: The System Council adopted the Agenda, as issued on 18 October 2017.
+Date(s): 9-10 November 2017
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row230]
+Decision: The System Council adopted the Agenda issued on 2 May 2018 (meeting document SC6-01).
+Date(s): 16 May 2018
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row195]
+Decision: The System Council extended the membership term of Daniel van Gilst, System Council voting member, Norway, for the System Council’s Assurance Oversight Committee (‘AOC’) until 30 June 2021.
+Date(s): 15-16 May 2019
+---
+[ID: pdf:SC17-16_MeetingSummary_Approved_.pdf:p23pt1]
+Meeting Summary: 17th System Council Meeting 17th System Council Meeting SC17-16 2-3 November 2022, Brisbane, Australia Page 23 of 32 i. Nikita Eriksen-Hamel (Canada) ii. Gary Jahn (USA) iii. Fatma Sarsu (Türkiye) b. Retroactively extends the terms of all other members of SIMEC until 30 June 2023 or such time as a successor is appointed. 83. Decision SC/M17/DP7 - AOC Membership Appointments Pursuant to paragraph 7 of the terms of reference of the System Council’s Assurance Oversight Committee, the System Council: a. Appointed Flora Mak (Canada) and Sarah Schmidt (Germany) as members of the Assurance Oversight Committee (‘AOC’) until 30 June 2023 or such time as their successors are appointed; and b. Retroactively extended the term of Muriel Uzán as a member of the AOC until 30 June 2023 or such time as a successor is appointed.
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row97]
+Decision: Pursuant to paragraph 7 of the terms of reference of the System Council’s Assurance Oversight Committee, the System Council appointed Fayezul Choudhury and Rita O’Sullivan as independent members of the Assurance Oversight Committee (‘AOC’) until 30 June 2023, or such time as their successors are appointed.
+Date(s): 15 February 2023
+---
+[ID: pdf:SC17-16_MeetingSummary_Approved_.pdf:p1pt2]
+Council Meeting 2-3 November 2022 Purpose: This document presents the formal meeting summary for the System Council’s 1 7th meeting (‘SC17’), as approved by the System Council on a no
+---
+[ID: pdf:SC17-16_MeetingSummary_Approved_.pdf:p23pt2]
+such time as their successors are appointed; and b. Retroactively extended the term of Muriel Uzán as a member of the AOC until 30 June 2023 or such time as a successor is appointed. Agenda Item 9: System Board and System Council responsibilities 84. In framing the session, t he session Chair indicated that, upon the System Board’s request, the System Council is being invited to reflect on a proposal to establish a small, joint cross -functional group to e xplore perceptions of inefficiencies and duplication across mandates, in a pragmatic and time-bound way. It was further noted that this was intended to be a discussion to consider incremental changes , versus fundamental transformation to the governing structure's architecture. 85. The Board Chair noted the Board’s awareness that there may be views of several System Council members
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row225]
+Decision: The System Council approved the document titled ‘Meeting Summary, 6th System Council meeting’ dated 1 October 2018
+Date(s): 30 October 2018
+---
+[ID: pdf:SC18-17_MeetingSummary_APPROVED.pdf:p10pt1]
+Meeting Summary: 18th System Council Meeting 18th System Council Meeting SC18-17 11-12 May 2023, Washington, DC, USA Page 10 of 42 (SPIA), pursuant to paragraph 6.6 of the SPIA terms of reference (TOR); b. Authorized SPIA to receive additional budget allocations through a flexible funding mechanism to supplement the pooled funding for the committed multi- year budgets; and c. Endorsed the revised SPIA TOR, pursuant to Articles 6.1 e) of the CGIAR System Framework. Agenda Item 5: Assurance and Oversight Committee (AOC) 26. At the invitation of the Co-Chair, the interim AOC Chair presented the AOC’s reflections and conclusions on the comprehensive review of the TOR, conducted in response to the Council’s request in November (SC17). 27. The presentation outlined the rationale for establishing the AOC as a standing committee of the Council and emphasized
+---
+[ID: pdf:SC22-Resource_SC-Action-Tracker.pdf:p1pt1]
+Update on actions agreed with the System Council Purpose: This additional resource for
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row92]
+Decision: The System Council adopted the Agenda, as re-issued on 27 April 2023, with revised timings.
+Date(s): 12 May 2023
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row63]
+Decision: The System Council approved the Integrated Partnership Board Member Profile as presented by the Nominations Committee of the System Council.
+Date(s): 8 May 2024
+---
+[ID: pdf:SC22-14_AOC Report to SC22.pdf:p3pt2]
+opinion and the IPB -AFRC Chair is not aware of any qualified opinions received for any Center.1 7. The AOC appreciates the support of the IPB -AFRC and System Council in resolving the matters raised in the SC Action Plan and related investigations. The AOC has worked closely with the Office of Ethics and Business Conduct in overseeing various investigations and has benefited from the support of a non-conflicted consultant. 8. Ensuring that gaps in the CGIAR Charter and Framework – as raised by AOC – are effectively resolved will be an important workstream during the proposed Q3 revision sessions. AOC oversight of the System Council Action Plan and related matters 9. In 2025, the AOC continued its work to close the remaining items of the System Council’s Action Plan. To date, 11 of the 12 matters have been closed. For the remaining item on remuneration of governance officials, a review is being overseen by the Nominations Committee of the System Council, with
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row53]
+Decision: Consensus was reached to endorse the slate of Integrated Partnership Board members as recommended by the Nominations Committee of the System Council (five rolling over members and seven new members).
+Date(s): 24 July 2024
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row40]
+Decision: Pursuant to Article C. 7 of  AOC’s Terms of Reference, the System Council approves the establishment of an Ad Hoc Nominating Committee to identify and recommend for approval a candidate for the position of independent member of the Assurance and Oversight Committee that shall be made up of the current members of the AOC and a representative from the System Council
+Date(s): 1 November 2024
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row47]
+Decision: Pursuant to the authority as delegated to the System Council by the System Board under its role pursuant to Article 7.6 of the Charter of the CGIAR System Organization (System Board decision reference SB/M28/EDP1), the System Council:
+- Appointed the following persons to the Integrated Partnership Board for an initial term of three years from 1 October 2024 to 30 September 2027: Nicholas Austin; Ramesh Chand; Rachel Chikwamba; Jessica Fanzo; Segenet Kelemu; Mauricio Lopes; Celso Moretti; Dhesigen Naidoo; Enrica Porcari;
+- Reappointed the following persons to the Integrated Partnership Board for an additional term from 1 October 2024: Lindiwe Majele Sibanda (to 30 September 2027); Patrick Caron (to 30 September 2026); Alice Ruhweza (to 30 September 2026); Shenggen Fan (to 30 September 2026); Clarissa van Heerden (to 30 September 2026.
+Date(s): 27 September 2024
+---
+[ID: pdf:SC-adhoc-20December2023_MeetingSummary-APPROVED.pdf:p3pt2]
+implementation. 8. In their interventions, System Council members were unanimous in their endorsement of the package of proposals in the Memorandum, and in their commendation of the Ad Hoc Committee on Governance for its stewardship of a constructive, collaborative and inclusive process to deliver an outcome and decision-making by the end of 2023. 9. Several System Council members called for additional detail to be provided around the intended role and responsibilities of the General Assembly of Centers, and its specific accountabilities in relation to the Integrated Partnership Board and the System Council. In particular, clarity was sought on its responsibilities relating to governance as well as being a forum for cross-Center interaction. (See action point SC19X-AP1) 10. Appreciation was expressed for the AOC’s
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row98]
+Decision: Pursuant to paragraph 9 of the terms of reference of the System Council’s Strategic Impact, Monitoring &amp; Evaluation Committee, the System Council appoints Dr. Didem Kökden as member of SIMEC until 30 June 2023 or such time as a successor is appointed.
+Date(s): 15 February 2023
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row255]
+Decision: The System Council approves the Terms of Reference for the Chair of SIMEC, as issued on 11 July 2017.
+Date(s): 19 July 2017
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row37]
+Decision: The System Council adopted the Agenda for the 21st System Council meeting, as issued on 27 November 2024.
+Date(s): 11-12 December 2024
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row137]
+Decision: The System Council adopted the Agenda as issued on 1 December 2021  (document SC14-01) .
+Date(s): 15 December 2021
+---
+[ID: pdf:SC-adhoc-20December2023_MeetingSummary-APPROVED.pdf:p1pt2]
+document presents the summary of an ad hoc System Council meeting held on 20 December 2023, including decisions taken and agreed actions from the meeting. I t was approved by the System Council on a no objection basis with effect from Thursday 18
+---
+[ID: pdf:SC18-17_MeetingSummary_APPROVED.pdf:p21pt1]
+Meeting Summary: 18th System Council Meeting 18th System Council Meeting SC18-17 11-12 May 2023, Washington, DC, USA Page 21 of 42 establishment of clear roles and accountabilities; j. The need to clearly define the tasks and accountabilities between the two governing bodies, with the aim of addressing some open questions that still exist following the change management process; and k. The need for the Council to be involved in important topics such as the renaming of CGIAR and the process of appointing System Board members. Input into the Process l. Insistence on keeping the Council fully engaged and consulted on key milestones and outputs and recommendations from the unified governance review; m. Advocacy for transparency and inclusivity, involving relevant stakeholders; n. The need for clarity on post-report next steps
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row32]
+Decision: Further to the System Council Action Plan issued on 10 September 2024, the System Council endorsed the status update report on the AOC’s oversight of that Action Plan provided as a pre-read for the System Council’s 21st meeting.
+Date(s): 11-12 December 2024
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row52]
+Decision: The System Council endorsed two additional candidates for membership of the Integrated Partnership Board  as recommended by the Nominations Committee of the System Council.
+Date(s): 8 August 2024
+---
+[ID: pdf:SC20_Chairs-Summary.pdf:p2pt3]
+as trees and agroforestry was encouraged. Underpinning CGIAR’s science and innovations, the Council heard substantive updates on the implementation of the new, integrated governance arrangements approved in December 2023. The Council welcomed the efforts of its Nominations Committee to wards the identification and appointment of a diverse, high -caliber Integrated Partnership Board (IPB). The Council approved the Committee’s revised timeline of next steps and looked forward to taking final appointment decisions in July 2024. As it prepares to appoint the IPB, the Council recognized the need for transparency and clarity on the responsibilities, accountabilities, and authorities of the new Board. To that end, Council members welcomed the joint System Council-System Board Working Group on the respective roles of the Integrated Partnership Board and the System Council. Beyond governance roles and responsibilities, the Council took note of the work of the ICI (Integrated, Coordinated,
+---
+[ID: pdf:SC22-14_AOC Report to SC22.pdf:p1pt2]
+December 2024 – May 2025 Purpose As a standing committee of the System Council, t his document sets out a summary of the Assurance Oversight Committee’s (AOC) activities and recommendations from December 2024 to May 2025. Action Requested The System Council is requested
+---
+[ID: pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p2pt2]
+the System Council (“Council”) held on 20 July 2022 as a virtual meeting. By way of overview: • Format. The meeting was held as a virtual meeting over a single session. • Agenda items. The meeting covered agenda items
+---
+[ID: pdf:SC21-16_Meeting Summary_Approved.pdf:p47pt1]
+Meeting Summary: 21st System Council Meeting 21st CGIAR System Council Meeting SC21-16 11-12 December 2024, Berlin, Germany Page 47 of 51 Key Discussion Areas 191. The Following member reflections were provided: a. Genebanks: A member raised a concern about the absence of a specific reference to Genebanks in the decision on the 2025–2030 Science and Innovation Portfolio. Management confirmed they would consult with the IPB during its February 2025 meeting and provide an update to Council. b. Internal Audit and Ethics: A request was made for further clarity on the scope and budget of internal audit and ethics functions. Management committed to providing an update to Council by mid-February, following the
+---
+[ID: pdf:SC21-16_Meeting Summary_Approved.pdf:p22pt4]
+November 2024 reviews of the Program and Accelerator proposals and Portfolio Narrative. 82. Action Point SC/M21/AP1 — CGIAR’s 2025-2030 Science and Innovation Portfolio The System Council requested that management consider the feedback provided by Council members on the intended governance and management arrangements for a Breeding for Tomorrow and Genebanks Science Program and provide a response by February 2025. Closed Session 83. The Council entered a closed session to receive and discuss the report of the Council’s Assurance Oversight Committee to the System Council Action Plan. Pursuant to Article 4.3(b) and (d) of the Rules of Procedure of the System Council, the Chair clarified attendance rules noting that attendance was limited to voting members of the System Council and one alternate.
+---
+[ID: xlsx:CGIAR System Council Decisions.xlsx:row132]
+Decision: The System Council approved the appointment of the following membership of the Strategic Impact, Monitoring and Evaluation Committee to 30 June 2022, unless earlier determined by the System Council: 
+•	Dougou Keita (African Development Bank) 
+•	Bethany Davies (Australia) 
+•	Ruben Echeverría (Bill &amp; Melinda Gates Foundat</t>
+  </si>
+  <si>
     <t>[{"role": "system", "content": "You are a helpful assistant that answer user questions in a detailed and comprehensive way.\n\nAlways base your answer strictly on the provided context.\nProvide a detailed and comprehensive answer to the question.\nAfter the answer, add a section 'Used Sources:' followed by a comma-separated list of the IDs from the chunks you used in formulating the answer (e.g., pdf:doc1.pdf:p1pt1, docx:doc2.docx:u1-4). Only list chunks that directly contributed. Do not make up IDs."}, {"role": "user", "content": "Question: What are the decisions from desicion register?\n\nContext:\n\n---\n\n[ID: pdf:SC22-08 - Governance Updates.pdf:p7pt2]\nLink: N/A\nFile: SC22-08 - Governance Updates.pdf\nLocation: page 7 part 2\nContent: gathering facts, analyzing information and preparing a proposal for the final decision-maker, and obtaining the required advice, clearances, and concurrences. Concur Responsible for\n\n---\n\n[ID: pdf:SC22-01_Agenda-Adopted.pdf:p1pt3]\nLink: N/A\nFile: SC22-01_Agenda-Adopted.pdf\nLocation: page 1 part 3\nContent: d. Declarations of interest(s) on the Agenda SC22-01, this document Resources: • Decisions taken out of session since SC21; • Action tracker b. For decision c. For adoption d. Action as needed 09:15-09:40 25 mins 2 Reflections from the Integrated Partnership Board Chair SC22-02 Presentation to the meeting For\n\n---\n\n[ID: pdf:SC22-20_Meeting Summary_Approved.pdf:p1pt4]\nLink: N/A\nFile: SC22-20_Meeting Summary_Approved.pdf\nLocation: page 1 part 4\nContent: Summary (reissued 4 July 2025) that confirmed decisions taken and actions agreed during the meeting (as also reproduced in this full meeting summary for completeness). Distribution notice: This document may be distributed\n\n---\n\n[ID: pdf:SC22-08 - Governance Updates.pdf:p3pt2]\nLink: N/A\nFile: SC22-08 - Governance Updates.pdf\nLocation: page 3 part 2\nContent: with Risk &amp; Oversight Plan and address the AOC’s comments iii. Policy development and adoption process (to align with Internal Rules Framework once finalized) iv. Whether two documents are really required – given high degree of duplication so that each can be read separately v. Differentiation between IFA-signatory Centers and non-IFA-signatory Centers vi. Process\n\n---\n\n[ID: pdf:SC17-16_MeetingSummary_Approved_.pdf:p1pt4]\nLink: N/A\nFile: SC17-16_MeetingSummary_Approved_.pdf\nLocation: page 1 part 4\nContent: Summary (issued 6 November 2022) that confirmed decisions taken and actions agreed during the meeting. Distribution notice: This document may be distributed without restriction. Prepared by: System Council Secretariat\n\n---\n\n[ID: pdf:SC-adhoc-20December2023_MeetingSummary-APPROVED.pdf:p1pt3]\nLink: N/A\nFile: SC-adhoc-20December2023_MeetingSummary-APPROVED.pdf\nLocation: page 1 part 3\nContent: on a no objection basis with effect from Thursday 18 January 2024 (Decision Reference SC/M19/EDP4). Basis of preparation: Pursuant to Article 9.2(a) of the System Council Rules of Procedure, the Secretariat shall not produce a verbatim record of proceedings. The following document therefore\n\n---\n\n[ID: pdf:SC22-20_Meeting Summary_Approved.pdf:p24pt4]\nLink: N/A\nFile: SC22-20_Meeting Summary_Approved.pdf\nLocation: page 24 part 4\nContent: the amendments process will address unresolved issues like the Council’s role in appointing and removing voting IPB members, as well as aligning language with the new ROP. Some concerns about the governance processes remain, particularly regarding the Council’s involvement in policy development and the risks of requiring unanimous Cent er approval for all the partnership policy documents. 76. The development of an Internal Rules Framework requires timely amendments to the Charter and Framework, as these documents define the approval roles of the IPB and System Council regarding policy adoption. The General Legal Counsel explained the long delay in developing the Internal Rules Framework. 77. Information was provided on the reconstituted G overnance Working Group, which will develop proposed changes with stakeholder consultation, aiming for dra ft governing documents for approval by the end of September, but allowing for longer-term follow-up if\n\n---\n\n[ID: pdf:SC22-08 - Governance Updates.pdf:p3pt3]\nLink: N/A\nFile: SC22-08 - Governance Updates.pdf\nLocation: page 3 part 3\nContent: be read separately v. Differentiation between IFA-signatory Centers and non-IFA-signatory Centers vi. Process for admission of new Centers vii. Amendments to CGIAR’s mission/purpose statements, definition of CGIAR Partners viii. Need for a detailed framework/process documentation on several topics, including dispute resolution; mechanisms for collaboration; board performance and accountability; IPB interface with Center Boards ix.\n\n---\n\n[ID: pdf:SC21-16_Meeting Summary_Approved.pdf:p45pt4]\nLink: N/A\nFile: SC21-16_Meeting Summary_Approved.pdf\nLocation: page 45 part 4\nContent: Close Consent Agenda 185. The acting Chair introduced the consent agenda items, which were presented by the Council Secretary. 186. According to Article 7.1(a) of the System Council ’s Rules of Procedure, which are for adoption as a package by the Council without discussion, the Council Secretary confirmed that no requests to remove any item from the consent agenda had been received by the relevant period, and thus the consent agenda was being put up for approval. The Council approved the items on the consent agenda without objection. 187. Decision Point — SC/M21/DP8 – System Council Rules of Procedure The System Council approved amendments to the Rules of Procedure of the System Council, in the form dated 27 November 2024, pursuant to paragraph 14.4 of those Rules of\n\n---\n\n[ID: pdf:SC22-08 - Governance Updates.pdf:p7pt3]\nLink: N/A\nFile: SC22-08 - Governance Updates.pdf\nLocation: page 7 part 3\nContent: and concurrences. Concur Responsible for reviewing the entire proposal. Without an agreement from the Concurrer, the proposal cannot be sent to the final\n\n---\n\n[ID: pdf:SC19-23_MeetingSummary-Approved.pdf:p39pt4]\nLink: N/A\nFile: SC19-23_MeetingSummary-Approved.pdf\nLocation: page 39 part 4\nContent: priorities, impact, finance, and assurance; and f. Further definition of partner country roles, not just host country, but partner country roles in governance, such as, for example, providing input to the slate of potential System Board Members. 170. In summary, he conveyed optimism about securing pivotal agreements within the current year and transitioning towards the effective implementation of governance changes in 2024. The Ad Hoc Committee on Governance is set to formulate a procedural plan, with a dedicated drafting group assigned to refine the language, aiming for the completion of an initial draft agreement by mid -November. He underscored the anticipation of formal approval by mid -December, indicating potential modifications to governing documents either by the end of this year or in the early months of the next, contingent upon the finalization of the agreement.\n\n---\n\n[ID: pdf:SC22-06a - Incentives WG - Inception Report with Annexes.pdf:p39pt4]\nLink: N/A\nFile: SC22-06a - Incentives WG - Inception Report with Annexes.pdf\nLocation: page 39 part 4\nContent: Council Seat Arrangements and Rules Value Proposition: • Proposal to frame Window 1 as mission-critical • Further discussion and refinement of the value proposition\n\n---\n\n[ID: pdf:SC22-08 - Governance Updates.pdf:p3pt1]\nLink: N/A\nFile: SC22-08 - Governance Updates.pdf\nLocation: page 3 part 1\nContent: Framework and Charter Feedback documented for consideration in this next amendment process (summarized, non-exhaustive) 1 i. Roles of the System Council relating to IPB appointments ii. Refine roles/responsibilities relating to internal audit, external audit, ethics and risk management/internal controls to align with Risk &amp; Oversight Plan and address the AOC’s comments iii. Policy development\n\n---\n\n[ID: pdf:SC22-20_Meeting Summary_Approved.pdf:p25pt2]\nLink: N/A\nFile: SC22-20_Meeting Summary_Approved.pdf\nLocation: page 25 part 2\nContent: challenges that will require further attention. Key Discussion Areas 80. Meeting participants expressed their appreciation for the presentation and its relevance to the CGIAR System. a. Clarification was sought on the approval process , whether unanimous approval is needed from the governing bodies on issues. b. The current absence of an I nternal Rules Framework is a contributing factor to uncoordinated decision -making and inefficiencies, underscoring the urgent need to implement this document. Concern was expressed over the delays caused by repeated delegation to working groups, and a call for a more ambitious time and streamlined process to move the effort forward was made. c. Also highlighted was the workload and necessary expertise burden placed on Council members through the multitude of ad hoc working groups, which is problematic, with a request to reconsider this approach to utilize specific expertise and resources better. d. The technical and political dimensions of finalizing the\n\n---\n\n[ID: pdf:SC17-16_MeetingSummary_Approved_.pdf:p4pt4]\nLink: N/A\nFile: SC17-16_MeetingSummary_Approved_.pdf\nLocation: page 4 part 4\nContent: 7. Formally tabling the provisional a genda, t he Chair made note of the Secretariat’s communication on the eve of the meeting, sharing the re-ordering of several items , adding an additional item 14a, and making space for some voices of the scientists. No declarations of interest were made on the agenda, and no items of other business were requested. The Chair confirmed that he would be flexible if additional areas arose during the meeting. 8. Decision SC/M17/DP2: Adoption of the Agenda The System Council adopted the Agenda, as re -issued on 2nd November 2022 with revised timings and an additional item 14a titled ‘Capturing our messaging’.2 1 Composition: https://www.cgiar.org/how-we-work/governance/system-council/sc-composition/ 2 The agenda was adopted pursuant to Article 7.2(a) of the System Council Rules of Procedure\n\n---\n\n[ID: pdf:SC22-08 - Governance Updates.pdf:p7pt4]\nLink: N/A\nFile: SC22-08 - Governance Updates.pdf\nLocation: page 7 part 4\nContent: be sent to the final decision-maker. Approve Responsible for considering the entire proposal and making a decision – and accountable for that decision.\n\n---\n\n[ID: pdf:Item 16 Presentation - SO 2024 Financial Statements.pdf:p1pt4]\nLink: N/A\nFile: Item 16 Presentation - SO 2024 Financial Statements.pdf\nLocation: page 1 part 4\nContent: Council for approval, following concurrence of the Integrated Partnership Board. Prepared by: Director, Business Operations and Finance\n\n---\n\n[ID: pdf:SC22-14-Annex - AOC Revised TOR.pdf:p4pt3]\nLink: N/A\nFile: SC22-14-Annex - AOC Revised TOR.pdf\nLocation: page 4 part 3\nContent: from their service, except in cases of gross negligence, willful misconduct, or fraudulent behavior. F. Declarations of Interests and Independence 1. Principle of Integrity: All AOC members must declare potential conﬂicts of interest, in line with a clear process for such disclosures. Independent members will annually sign declarations of independence to ensure the Committee’s decisions remain objective and free from undue inﬂuence. 2. Principle of Conﬁdentiality: AOC shall maintain the conﬁdentiality of all non-public information received, reviewed, or discussed in the course of their duties. All conﬁdential documents and information submitted or obtained by AOC shall remain conﬁdential . AOC members shall not disclose such information\n\n---\n\n[ID: pdf:F2R-CWANA.pdf:p49pt1]\nLink: N/A\nFile: F2R-CWANA.pdf\nLocation: page 49 part 1\nContent: 49 registration process. Outcome IO 2.02 Global Genetic Innovation Initiatives develop Product Profiles that are specifically targeted to the requirements of stakeholders in CWANA. Number of beneficiaries using the innovation, disaggregate d by gender Number EG, LB, MA, SD, UZ Primary Key informant interviews; Stakeholder consultations Annual Not availabl e Not availabl\n\n---\n\n[ID: pdf:SC22-07a - ROP - Status Report to SC22.pdf:p1pt4]\nLink: N/A\nFile: SC22-07a - ROP - Status Report to SC22.pdf\nLocation: page 1 part 4\nContent: Decision-making processes on one item – the Ethics &amp; Business Conduct Escalation Framework – was paused and is undergoing further review at the date of issue of this document, following feedback received from the AOC. An update on the finalization of that document will be provided during the meeting session. At the date of issue of this document, decision-making is ongoing during Center AFRC and Board meetings as part of the Q2 meetings cycle. The status of some approvals is therefore expected to change between the issue of this document and the date of the System Council’s 22nd meeting – and an update will be provided during the\n\n---\n\n[ID: pdf:SC20-19_Meeting Summary_APPROVED.pdf:p2pt4]\nLink: N/A\nFile: SC20-19_Meeting Summary_APPROVED.pdf\nLocation: page 2 part 4\nContent: sequence in this summary. Participants: Annex 1 sets out a list of meeting participants. Basis of preparation: Pursuant to Article 9.2(a) of the System Council Rules of Procedure , the Secretariat shall not produce a verbatim record of proceedings. The following document therefore neither attributes interventions, nor reproduces direct quotes of any individual System Council member, Active Observer, or other invited\n\n---\n\n[ID: pdf:SC22-20_Meeting Summary_Approved.pdf:p36pt2]\nLink: N/A\nFile: SC22-20_Meeting Summary_Approved.pdf\nLocation: page 36 part 2\nContent: of the System Council 123. The Nominations Committee of the System Council (NCSC) Co-Chair of the NCSC, presented updates, including: a. NCSC composition, which is comprised of 11 members (including one independent member). There is currently a vacancy for one member to be nominated by the Council. b. The NCSC initiated an honorarium benchmarking exercise in November 2024 using both quantitative and qualitative methods. The review also encompasses the travel policy to ensure a holistic evaluation, with the draft report scheduled for completion by the end of June and the final report expected by mid-July. c. Work is underway to develop and present to the C ouncil for approval the key performance indicators against which the NCSC would evaluate the IPB with inputs from the General Assembly of Centers. d. The NCSC’s responsibilities extend beyond presenting potential IPB nominees to Council for approval. The NCSC Co-Chair indicated that\n\n---\n\n[ID: pdf:SC21-16_Meeting Summary_Approved.pdf:p35pt2]\nLink: N/A\nFile: SC21-16_Meeting Summary_Approved.pdf\nLocation: page 35 part 2\nContent: Integrated Partnership ROP, reviewing the amendments to the Charter and Framework, and overseeing the Action Plan approved by the SC on September 5 that dealt with key issues stemming from the 45 red flags letter. 136. Mr. Seligmann provided an update on AOC’s findings related to the Action Plan. He presented the ongoing efforts focused on the three remaining items: i) resolving the investigation into the dismissal of a senior scientist by CIMMYT through engagement with its Board of Trustees; ii) finalizing the investigation into the independence of the Ethics and Business Conduct functio n, which is nearing completion; and iii) the item related to the remuneration of governance officials. For item iii he indicated that this is under the aegis of the Nominations Committee of the System Council , which will oversee a benchmarking exercise and make recommendations to the System Council. 137. Mr.\n\n---\n\n[ID: pdf:Asian-Mega-Deltas.pdf:p68pt2]\nLink: N/A\nFile: Asian-Mega-Deltas.pdf\nLocation: page 68 part 2\nContent: ● Annex 2.4: Priority setting: Further details ● Annex 2.6.1: Letters of support ● Annex 2.6.2: AMD country strategies and priorities ● Annex 2.6.3: Ongoing\n\n---\n\n[ID: pdf:SC22-20_Meeting Summary_Approved.pdf:p25pt4]\nLink: N/A\nFile: SC22-20_Meeting Summary_Approved.pdf\nLocation: page 25 part 4\nContent: explaining that efforts were paused due to other governance priorities. She indicated that the document is nearly complete but requires full agreement from all Centers , as outlined in the Integration Framework Agreement. For amendments to the Framework and Charter, a two-thirds majority from the General Assembly of Centers is sufficient for approval. f. The General Legal Counsel presented the composition and structure of the Governance Working Group as another way to achieve the technical and political aspects of the process. She indicated that the drafting team, made up mostly of internal experts from the System Organization and Centers , will handle the technical work on the I nternal Rules Framework. However, political guidance and decisions are crucial, since technical solutions alone won’t ensure success without broader political support. g. Commenting also on the process , IPB Representative on the Governance Working Group highlighted that achieving political consensus may require additional steps\n\n---\n\n[ID: pdf:SC22-01_Provisional-Agenda Annotated.pdf:p1pt4]\nLink: N/A\nFile: SC22-01_Provisional-Agenda Annotated.pdf\nLocation: page 1 part 4\nContent: c. Provisional Agenda and confirmation of quorum – for adoption d. Declarations of interest(s) on the Agenda – action as needed SC22-01, this document 09:15- 09:40 25 mins 2 Reflections from the Integrated Partnership Board Chair – for information No pre-reads 09:40- 10:00 20 mins 3 Reflections from the Executive Managing Director – for information No pre-reads\n\n---\n\n[ID: pdf:Resilient-Aquatic-Food-Systems.pdf:p5pt3]\nLink: N/A\nFile: Resilient-Aquatic-Food-Systems.pdf\nLocation: page 5 part 3\nContent: Advisory Michael Phillips M CGIAR Advisory Nicolette Duncan F CGIAR Core writing team Nitya Rao F University of East Anglia Advisory Petra Schmitter F World Bank Advisory Philippa Cohen F CGIAR Advisory Quennie Rizaldo F CGIAR Advisory Rahma Adam F CGIAR Advisory Robyn Johnston F ACIAR Advisory Rodolfo Dam Lam M CGIAR Advisory Rodrigue Yossa M CGIAR Advisory Rohana Subasinghe F CGIAR Advisory Sanjiv de Silva M CGIAR Advisory Sarah Freed F\n\n---\n\n[ID: pdf:SC22-08 - Governance Updates.pdf:p4pt3]\nLink: N/A\nFile: SC22-08 - Governance Updates.pdf\nLocation: page 4 part 3\nContent: to provide the opportunity to raise any concerns given the changed roles for those stakeholders in the proposed IRF. • Two key points of feedback were received: i) on consequences of the changed role of the System Council relating to policy approval; and ii) concerns over unanimity of approvals by Centers giving an effective veto power. • At its 11-12 April meeting, the IPB recognized the need for additional consultation with Centers and the System Council to further consider the policy approval mechanism set out in\n\n---\n\n[ID: pdf:SC20-19_Meeting Summary_APPROVED.pdf:p22pt3]\nLink: N/A\nFile: SC20-19_Meeting Summary_APPROVED.pdf\nLocation: page 22 part 3\nContent: or responsibility, ensuring clear lines of accountability. This empowers both the SC and IPB to perform effectively, each with a clear comparative advantage in its respective roles d. They outlined a process with three key roles: ‘recommend ’ (gather facts, prepare proposals), ‘concur’ (review proposals and agree to advance them), and ‘approve’ (make the final decisions and be accountable for them ). Importantly, when concurrence is required, a proposal cannot proceed to the approval stage without agree ment from the concurring party. However, the final decision and full accountability rests with the designated approving body, ensuring clear responsibility for outcomes. e. To explain the relationship between the Council and IPB, they used a parliamentary metaphor: the Council as an ‘upper house ’ overseeing overall vision and strategy, and the IPB as a ‘lower house’ overseeing management and execution. f. They noted that a\n\n---\n\n[ID: pdf:SC18-17_MeetingSummary_APPROVED.pdf:p1pt4]\nLink: N/A\nFile: SC18-17_MeetingSummary_APPROVED.pdf\nLocation: page 1 part 4\nContent: 18 Chair’s Summary (issued 25 May 2023) that confirmed decisions taken and actions agreed during the meeting. Distribution notice: This document may be distributed without restriction. Prepared by: System Council\n\n---\n\n[ID: pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p1pt4]\nLink: N/A\nFile: SC16-07_Meeting-Summary-APPROVED.pdf\nLocation: page 1 part 4\nContent: decisions taken and agreed actions from the meeting. Distribution notice: This document is an internal working document of the CGIAR System and should not be publicly quoted until formally approved. Prepared by: System\n\n---\n\n[ID: pdf:SC19-23_MeetingSummary-Approved.pdf:p1pt4]\nLink: N/A\nFile: SC19-23_MeetingSummary-Approved.pdf\nLocation: page 1 part 4\nContent: the SC19 Chair’s Summary (issued 27 October 2023) that confirmed decisions taken and agreed actions during the meeting. Distribution notice: This document may be distributed without restriction. Prepared by: System Council Secretariat\n\n---\n\n[ID: pdf:SC-adhoc-20December2023_MeetingSummary-APPROVED.pdf:p4pt2]\nLink: N/A\nFile: SC-adhoc-20December2023_MeetingSummary-APPROVED.pdf\nLocation: page 4 part 2\nContent: • The outcomes of that independent external review, overseen by the Ad Hoc Committee on Governance, have been translated through a consultative process into a set of proposals by a Drafting Working Group drawn from across the IFA Parties and the System Council – in the form of the “CGIAR memorandum on the implementation of governance recommendations”; Now therefore, the System Council: • Endorsed the “CGIAR memorandum on the implementation of governance recommendations”; • Approved the package of proposals set out therein; and • Committed to working in good faith to take required decisions to achieve the Integrated\n\n---\n\n[ID: pdf:SC17-16_MeetingSummary_Approved_.pdf:p29pt4]\nLink: N/A\nFile: SC17-16_MeetingSummary_Approved_.pdf\nLocation: page 29 part 4\nContent: require formal System Council decision. The Secretary confirmed that no requests to remove any it em from the Consent Agenda had been received by the relevant period, and thus the Consent Agenda was being put up for approval . The System Council approved the consent agenda. 9 108. As a follow up to the discussion on gender, diversity and inclusion (‘GDI’), the System Council accepted the proposal from a System Council member that GDI be a standing item. 109. Action SC/M17/AP3: Gender, Diversity and Inclusion in CGIAR Gender, Diversity and Inclusion (‘GDI’) will be a standing agenda item for future System Council regular meetings, with a rotating area of specific focus in any given meeting. 9 Refer to ‘Decision SC/M17/DP5 - SPIA Membership Appointments’ under session outcomes of the SC17 SPIA agenda\n\n---\n\n[ID: pdf:SC22-08 - Governance Updates.pdf:p6pt4]\nLink: N/A\nFile: SC22-08 - Governance Updates.pdf\nLocation: page 6 part 4\nContent: drafts of all documents Consultation on drafts – providing good time for review and feedback Analysis of feedback; revision of drafts by GWG Iterative consultation process as required to ensure issues worked through before issuing versions for decision Approvals by the IPB, SC and GAC\n\n---\n\n[ID: pdf:SC19-23_MeetingSummary-Approved.pdf:p2pt4]\nLink: N/A\nFile: SC19-23_MeetingSummary-Approved.pdf\nLocation: page 2 part 4\nContent: in sequence in this summary. Participants: Annex 1 sets out a list of meeting participants. Basis of preparation: Pursuant to Article 9.2(a) of the System Council Rules of Procedure , the Secretariat shall not produce a verbatim record of proceedings. The following document therefore neither attributes interventions, nor reproduces direct quotes of an individual System Council member, Active Observer, or\n\n---\n\n[ID: pdf:SC18-17_MeetingSummary_APPROVED.pdf:p2pt4]\nLink: N/A\nFile: SC18-17_MeetingSummary_APPROVED.pdf\nLocation: page 2 part 4\nContent: in sequence in this summary. Participants: Annex 1 sets out a list of meeting participants. Basis of preparation: Pursuant to Article 9.2(a) of the System Council Rules of Procedure, the Secretariat shall not produce a verbatim record of proceedings. The following document therefore neither attributes interventions, nor reproduces direct quotes of an individual System Council member, Active Observer, or other invited\n\n---\n\n[ID: pdf:SC22-14-Annex - AOC Revised TOR.pdf:p5pt2]\nLink: N/A\nFile: SC22-14-Annex - AOC Revised TOR.pdf\nLocation: page 5 part 2\nContent: of 5 Approved: XXXXX H. Amendments The AOC will review these Terms of Reference every two\n\n---\n\n[ID: pdf:SC18-17_MeetingSummary_APPROVED.pdf:p23pt3]\nLink: N/A\nFile: SC18-17_MeetingSummary_APPROVED.pdf\nLocation: page 23 part 3\nContent: and inclusive integration of Centers not party to the Integrated Framework Agreement (IFA) into One CGIAR. Day 2 Opening 76. The Chair welcomed participants to the second day of the meeting, highlighting the focus on science and innovation. He invited Innocent Musabyimana to serve as the meeting Co-Chair for the day, in addition to recognizing his role as the representative for the AfDB. 77. Before proceeding to the planned agenda, the Chair addres sed two administrative matters. These included appointing a second Council representative to the Ad Hoc Committee on Governance and emphasizing the importance of assessing the current status and ensuring inclusive representation of the Council. Composition of the System Council going forwards 78. Decision SC/M18/DP6: System Council Representation on Ad Hoc Committee on Governance The System\n\n---\n\n[ID: pdf:SC21_Chair's Summary.pdf:p5pt2]\nLink: N/A\nFile: SC21_Chair's Summary.pdf\nLocation: page 5 part 2\nContent: for the System Council’s 21st meeting. SC/M21/DP8 – System Council Rules of Procedure The System Council approved amendments to the Rules of Procedure of the System Council, in the form dated 27 November 2024, pursuant to paragraph 14.4 of those Rules of Procedure. SC/M21/DP9 – System Council Chair Terms of Reference The System Council approved amendments to the Terms of Reference of the System Council Chair, in the form dated 27 November 2024, pursuant to Article 5.5 of the CGIAR System Framework. SC/M21/DP10 – Nominations Committee of the System Council The System Council approved the appointment of Dr. Cristina Rumbaitis del Rio, Vice -Chair, WorldFish Board of Trustees, to serve on the Nominations Committee of the System Council pursuant to Article 8.3 of the CGIAR System\n\n---\n\n[ID: pdf:SC-adhoc-20December2023_MeetingSummary-APPROVED.pdf:p2pt3]\nLink: N/A\nFile: SC-adhoc-20December2023_MeetingSummary-APPROVED.pdf\nLocation: page 2 part 3\nContent: is asked at this time to endorse the Memorandum and approve the package of proposals set out therein – and commit to working in good faith to take required decisions to achieve the Integrated Partnership by the dates set out in the Memorandum. He acknowledged the thoughtful advice of the Council’s Assurance Oversight Committee in support of the Council’s decision - making, including areas that the Council should prioritize as implementation is taken forward. 5. The Chair invited Dr. Kanayo F. Nwanze, Co -Chair of the Ad Hoc Committee on Governance, to provide an overview of the process and the recommendations. Dr. Nwanze recalled the highly consultative process followed since work commenced in Q2 2023, which included a multistakeholder webinar, in-person workshop and a series of working sessions. He reflected that the package of\n\n---\n\n[ID: pdf:SC18-17_MeetingSummary_APPROVED.pdf:p22pt2]\nLink: N/A\nFile: SC18-17_MeetingSummary_APPROVED.pdf\nLocation: page 22 part 2\nContent: ongoing System Framework and Charter amendment process, with any changes requiring approval from the Board, the Council, and a two -thirds majority of the General Assembly of Centers , and with the disadvantage of potentially forcing a decision before a Center is ready ; Option 2 suggest ed waiting for the unified governance review to be completed before revisiting the topic, with the disadvantage of persisting ambiguities that could impact the development of the 2025 -2027 portfolio; Option 3 proposed seeking a voluntary withdrawal by the Centers from the Framework, which would eliminate the need to terminate the Framework or make changes to definitions. 69. The Global General Counsel conveyed the Board’s preference for a diplomatic resolution, while acknowledging that the pursuit of CIFOR -ICRAF and ICRISAT ’s participation as signatories to the\n\n---\n\n[ID: pdf:SC22-08 - Governance Updates.pdf:p6pt3]\nLink: N/A\nFile: SC22-08 - Governance Updates.pdf\nLocation: page 6 part 3\nContent: Q3 to address these. May June July August September October Formation of Governance Working Group Consultation on IRF with stakeholder groups Collation/review of inputs on Charter/Framework (from last amendments and reflections since) Preparation of revised drafts of all documents Consultation on drafts – providing good time\n\n---\n\n[ID: pdf:SC18-17_MeetingSummary_APPROVED.pdf:p11pt2]\nLink: N/A\nFile: SC18-17_MeetingSummary_APPROVED.pdf\nLocation: page 11 part 2\nContent: for updating the risk appetite statement to incorporate recent changes, including the IFA, additional CGIAR C enters joining One CGIAR, and the unified governance review. On Composition of AOC: g. Recognition of the importance of term limits and phased rotation as essential governance practices; h. Suggestions to implement three -year or four -year membership term limits, explore staggered timing of rotations (such as rotat ing one-third of the committee annually) and developing a clear succession plan; i. Commitment to exploring staggered timing of rotations and developing a clear succession plan; and j. Appreciation for the diverse expertise and perspectives of new independent AOC members in enhancing due diligence and advising the Council. Session Outcomes 31. The Co-Chair expressed appreciation\n\n---\n\n[ID: pdf:SC22-20_Meeting Summary_Approved.pdf:p35pt3]\nLink: N/A\nFile: SC22-20_Meeting Summary_Approved.pdf\nLocation: page 35 part 3\nContent: its requirement for a robust process to escalate systemic issues. Notable improvements in CGIAR governance, the recruitment of highly qualified executives, and the establishment of clearer mandates are fostering trust and gradually shifting the equilibrium. As these central functions become more effective, Centers are increasingly willing to rely on them for critical processes. 117. The IPB Vice Chair described the process as a valuable learning experience, noting that progress has been made in building trust, establishing confidence, and clarifying rules, which sets a positive foundation for moving forward. 118. The EMD emphasized the need to be realistic regarding committee approval timelines and suggested reducing bureaucracy in the future. She highlighted progress on the escalation framework and the approval of executive roles, stressing the importance of having highly qualified individuals to build trust. 119. The Council Chair emphasized the ongoing commitment to achieving the highest standards of oversight. He acknowledged the significant progress made,\n\n---\n\n[ID: pdf:SC22-01_Provisional-Agenda Annotated.pdf:p4pt2]\nLink: N/A\nFile: SC22-01_Provisional-Agenda Annotated.pdf\nLocation: page 4 part 2\nContent: 6.2.i) a. Status update on implementation – for information b. Update on finalization of the Ethics &amp; Business Conduct Escalation Framework – for information Presenters: Essam Mohammed (Convener of the DGs) and Juan Lucas Restrepo (ICI Committee Co-Convener) • Items a and b are for information, whilst items c and d are for decision. The AOC’s report to the System Council includes its advice relating to matters under this agenda item. Background to items a and b Document SC22-07a provides a status report on the implementation of the Integrated Partnership Risk &amp; Oversight Plan, detailing key deliverables, their current status, and next steps as of\n\n---\n\n[ID: pdf:SC20-19_Meeting Summary_APPROVED.pdf:p21pt3]\nLink: N/A\nFile: SC20-19_Meeting Summary_APPROVED.pdf\nLocation: page 21 part 3\nContent: Review (UGR) CGIAR Memorandum on the Implementation of Governance Recommendations. b. Following an in -depth consultation process that yielded 188 submissions of substantive input, the Working Group is incorporating feedback and preparing a document explaining the changes, including a table mapping the specific recommendation provisions to the proposed changes. 53. Center DGs in attendance shared reflections on the ICI process: a. Stressed that decision-making wil</t>
   </si>
   <si>
@@ -5123,6 +5499,9 @@
   </si>
   <si>
     <t>[{"role": "system", "content": "You are a helpful assistant that answer user questions in a detailed and comprehensive way.\n\nAlways base your answer strictly on the provided context.\nProvide a detailed and comprehensive answer to the question.\nAfter the answer, add a section 'Used Sources:' followed by a comma-separated list of the IDs from the chunks you used in formulating the answer (e.g., pdf:doc1.pdf:p1pt1, docx:doc2.docx:u1-4). Only list chunks that directly contributed. Do not make up IDs."}, {"role": "user", "content": "Question: What was management's response to the System Council's feedback on the governance of breeding programs and genebanks?\n\nContext:\n\n---\n\n[ID: pdf:SC22-Resource_SC-Action-Tracker.pdf:p2pt1]\nLink: N/A\nFile: SC22-Resource_SC-Action-Tracker.pdf\nLocation: page 2 part 1\nContent: Completed action from previous meetings (SC21) 1 Action SC/M21AP1 The System Council requested that management consider the feedback provided by Council members on the intended governance and management arrangements for a Breeding for Tomorrow and Genebanks Science Program and provide a response by February 2025. Management provided a response to SC on 3 March 2025, advising that: Drawing on the experience of the Genebanks Platform and\n\n---\n\n[ID: pdf:SC21-16_Meeting Summary_Approved.pdf:p46pt2]\nLink: N/A\nFile: SC21-16_Meeting Summary_Approved.pdf\nLocation: page 46 part 2\nContent: System Council pursuant to Article 8.3 of the CGIAR System Framework and paragraph 2.1.2 of t he Terms of Reference of the Nominations Committee of the System Council. Review of SC21 Council Decisions 190. The Council Secretary provided a detailed summary of key decisions and actions from the meeting, including: a. Adoption of the agenda and appointment of Jens Busma as Co -Chair for this meeting. b. Approval of the 2025-2030 Science and Innovation Portfolio , with a request for ISDC to conduct a targeted review of Inception Reports and Workplans/Budgets by Q3 2025. c. Request for management to respond by February 2025 to feedback on the proposed governance and management of the Breeding for Tomorrow and Genebanks Science Program. d. Approval of the Integrated Partnership Risk &amp; Oversight Plan and endorsement of the IPB-AFRC\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row68]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 68\nContent: Decision: Pursuant to Article 6.1 ff) of the CGIAR System Framework, the System Council endorsed the evaluation of the GENEBANK Platform, taking into account the Management Responses.\nDate(s): 5 March 2024\n\n---\n\n[ID: pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p14pt4]\nLink: N/A\nFile: SC16-07_Meeting-Summary-APPROVED.pdf\nLocation: page 14 part 4\nContent: for Monitoring Evaluation and Learning require continued attention and effort. 34. The Global Director, Genetic Innovation (a.i) summarized the Management Response to the evaluation, emphasizing that management appreciate s, welcomes and embraces the set of nine recommendations made, and adding that: a. Development of the response had been highly inclusive, enabled by One CGIAR, including all Centers and their breeding programs as well as colleagues beyond the genetic innovation space, such as the People &amp; Culture team; b. That all technical and managerial recommendations will be addressed; c. That where two recommendations were ‘Partially Accepted’, the only deviation from full acceptance is that whilst management recognizes and understands the evaluators’ focus on governance, it is proposed that governance mechanisms be established across the genetic innovation space as a more valuable and unified 6 Set out in more detail in the presentation available at: https://storage.googleapis.com/cgiarorg/2022/07/CAS-PPT-EiB-Platform-Evaluation-for-SC-drop-in- July2022.pdf\n\n---\n\n[ID: pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p14pt1]\nLink: N/A\nFile: SC16-07_Meeting-Summary-APPROVED.pdf\nLocation: page 14 part 1\nContent: Meeting Summary: 16th System Council Meeting 16th System Council Meeting SC16-07 20 July 2022, Virtual Page 14 of 19 evaluation of the Excellence in Breeding (EiB) platfor m and how its recommendations are being taken forward across CGIAR based on evidence of what is needed to reach ever higher in terms of performance, efficiency and effectiveness. He added that many System Council colleagues had benefitted from deep -dive sessions held prior to this meeting that provided additional opportunity to hear in more detail the evaluation’s recommendations and response. 32. The interim Chair of the Council’s Strategic Impact, Monitoring and Evaluation Committee (‘SIMEC’) provided reflections on behalf of SIMEC, noting: a. That while some challenges had been encountered in undertaking the evaluation, these had been handled thoughtfully and professionally by the Advisory Services Shared Secretariat and CGIAR’s Global Science Leaders, enabling the final report to be\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row202]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 202\nContent: Decision: The System Council approved the creation of an additional module in the ‘Excellence in Breeding Platform’ to facilitate targeted funding of the Crops to end Hunger Initiative.\nDate(s): 15-16 May 2019\n\n---\n\n[ID: pdf:SC17-16_MeetingSummary_Approved_.pdf:p11pt1]\nLink: N/A\nFile: SC17-16_MeetingSummary_Approved_.pdf\nLocation: page 11 part 1\nContent: Meeting Summary: 17th System Council Meeting 17th System Council Meeting SC17-16 2-3 November 2022, Brisbane, Australia Page 11 of 32 29. CGIAR’s Managing Director, Genetic Innovation, then gave a presentation on how the ambitions for Genetic Innovation as a globally integrated strategic program can only be achieved if CGIAR operates with integrated governance and management. Reiterating that ultimately this will be dependent on a coherent, innovative, systems- based portfolio, the Managing Director emphasized the importance of ensuring that: a. Center crop programs continue to provide key entry points for the private sector and policymakers; b. Genebanks and breeding teams in different Centers have a unified crop strategy (for example: global rice program); c. Breeding pipelines and teams work to demand -driven product profiles across CGIAR’s five (5) impact areas based on shared market segment analyses; d. There is coordination and costing of the full pipeline from\n\n---\n\n[ID: pdf:SC21-16_Meeting Summary_Approved.pdf:p47pt1]\nLink: N/A\nFile: SC21-16_Meeting Summary_Approved.pdf\nLocation: page 47 part 1\nContent: Meeting Summary: 21st System Council Meeting 21st CGIAR System Council Meeting SC21-16 11-12 December 2024, Berlin, Germany Page 47 of 51 Key Discussion Areas 191. The Following member reflections were provided: a. Genebanks: A member raised a concern about the absence of a specific reference to Genebanks in the decision on the 2025–2030 Science and Innovation Portfolio. Management confirmed they would consult with the IPB during its February 2025 meeting and provide an update to Council. b. Internal Audit and Ethics: A request was made for further clarity on the scope and budget of internal audit and ethics functions. Management committed to providing an update to Council by mid-February, following the\n\n---\n\n[ID: pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p32pt4]\nLink: N/A\nFile: INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf\nLocation: page 32 part 4\nContent: broad impact, in particular with breeding programs targeting biofortification (Section 6.1 C). Measuring performance and results WP 3 Outcomes 3.1 and 3.2: Increased use of genebank collections and data by breeders. WP 4: (all Outcomes): National programs capacity for conserving germplasm is enhanced; collecting missions; Key partners have increased capacity to implement and operate under international laws; Recognition/endorsement of Greenpass protocol by national programs (Section 6.1 C for metrics) Partners CGIAR trait development teams and breeders; IPPC, NPPOs; FAO, ITPGRFA , CBD; civil society organizations; the seed industry; universities , IARCs, national, regional, and international genebanks. Human resources and capacity development The required human resources and skills are already embedded in the staffing of the Initiative; no additional resources or\n\n---\n\n[ID: pdf:SC21-16_Meeting Summary_Approved.pdf:p22pt4]\nLink: N/A\nFile: SC21-16_Meeting Summary_Approved.pdf\nLocation: page 22 part 4\nContent: November 2024 reviews of the Program and Accelerator proposals and Portfolio Narrative. 82. Action Point SC/M21/AP1 — CGIAR’s 2025-2030 Science and Innovation Portfolio The System Council requested that management consider the feedback provided by Council members on the intended governance and management arrangements for a Breeding for Tomorrow and Genebanks Science Program and provide a response by February 2025. Closed Session 83. The Council entered a closed session to receive and discuss the report of the Council’s Assurance Oversight Committee to the System Council Action Plan. Pursuant to Article 4.3(b) and (d) of the Rules of Procedure of the System Council, the Chair clarified attendance rules noting that attendance was limited to voting members of the System Council and one alternate.\n\n---\n\n[ID: pdf:SC19-23_MeetingSummary-Approved.pdf:p17pt1]\nLink: N/A\nFile: SC19-23_MeetingSummary-Approved.pdf\nLocation: page 17 part 1\nContent: Meeting Summary: 19th System Council Meeting 19th System Council Meeting SC19-23 20-21 October 2023, Rabat, Morocco Page 17 of 45 Agenda Item 8: Funding CGIAR’s Genebanks 60. The Co-Chair introduced the genebank funding discussion, linking to the prior item on funding modalities. He recalled the prior day ’s message from Morocco ’s Minister of Agriculture on the challenge of doing more with less, emphasizing efficiency and impact as CGIAR aims to optimize limited resources. 61. The interim EMD reported a decrease in expected Crop Trust funding for CGIAR genebanks, prompting the use of W1 funds to fill the gap. Initially affecting the Genetic Innovation Science Group, future allocations will be deducted uniformly from the top, impacting all three Science Groups. Discussions on funding modalities are underway to secure a sustainable genebank funding solution in\n\n---\n\n[ID: pdf:SC21-16_Meeting Summary_Approved.pdf:p21pt4]\nLink: N/A\nFile: SC21-16_Meeting Summary_Approved.pdf\nLocation: page 21 part 4\nContent: CGIAR programs, such as those under climate action, to partner with NARES, to leverage their knowledge, understand the context and infrastructure available in the geographies where programs are implemented. 78. Council members also provided specific reflections for the individual Portfolio science Programs and Accelerators for leadership to consider during the inception phase , including calling for keeping the Genebanks as an asset held in trust under the International Treaty on Plant Genetic Resources for Food and Agriculture (Plant Treaty). Members emphasized the importance of maintaining Genebanks as independent entities with ringfenced funding to meet Plant Treaty obligations, distinct from the new Portfolio’s “Breeding for Tomorrow ” Program. They highlighted Genebanks as critical global resources held in trust, benefiting researchers and farmers beyond CGIAR. Concerns were raised about the risks of merging Genebanks with the “Breeding for Tomorrow” Program, including operational challenges and inflated budgets, and members urged thorough analysis before decisions are made.\n\n---\n\n[ID: pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p14pt2]\nLink: N/A\nFile: SC16-07_Meeting-Summary-APPROVED.pdf\nLocation: page 14 part 2\nContent: a. That while some challenges had been encountered in undertaking the evaluation, these had been handled thoughtfully and professionally by the Advisory Services Shared Secretariat and CGIAR’s Global Science Leaders, enabling the final report to be useful and valuable; and b. That the report’s recommendations ad dress several core issues in CGIAR as well as specifically in breeding programs , with a Management Re sponse that demonstrates commitment to address these holistically – and the evaluation is thus welcomed and recommended by SIMEC for System Council endorsement. 33. The Director, CGIAR Advisory Services Shared Secretariat added reflections, highlighting: a. That a primary mitigation measure for the challenges encountered had been a substantive validation phase following a process discussed and agreed with SIMEC – providing assurance to the System Council that evaluation industry standards have been thoughtfully reflected in the evaluation report; b. That the CGIAR\n\n---\n\n[ID: pdf:SC17-16_MeetingSummary_Approved_.pdf:p24pt4]\nLink: N/A\nFile: SC17-16_MeetingSummary_Approved_.pdf\nLocation: page 24 part 4\nContent: of that review by not later than 14 April 2023. Agenda Item 11: Independent Science for Development Matters 91. The System Council watched two final ‘lightening talk’ videos introduced by the EMD as ‘voices from the ground,’ to provide an introduction to a discussion on impact: a. Young Wha Lee , Lead of the Breeding Resources Initiative – who spoke about how more and better data supports breeders as they integrate innovative technologies into their work to support farmers by identifying the best varieties faster; and b. Michael Abberton, the Head of the Genebanks Resources Center at IITA and One CGIAR Convener in Sierra Leone – who spoke to how the Genebanks Initiative delivers impact now and in the future in the face of climate and other global challenges.\n\n---\n\n[ID: pdf:SC21_Chair's Summary.pdf:p5pt3]\nLink: N/A\nFile: SC21_Chair's Summary.pdf\nLocation: page 5 part 3\nContent: appointment of Dr. Cristina Rumbaitis del Rio, Vice -Chair, WorldFish Board of Trustees, to serve on the Nominations Committee of the System Council pursuant to Article 8.3 of the CGIAR System Framework and paragraph 2.1.2 of the Terms of Reference of the Nominations Committee of the System Council. ACTIONS AGREED SC/M21/AP1 – CGIAR’s 2025-2030 Science and Innovation Portfolio The System Council requested that management consider the feedback provided by Council members on the intended governance and management arrangements for a Breeding for Tomorrow and Genebanks Science Program and provide a response by February 2025. SC/M21/AP2 – Planning 2025 independent advising and evaluative evidence for the System Council The System Council requested that Terms of Reference be developed by end -Q1 2025, for System Council consideration and\n\n---\n\n[ID: pdf:SC19-23_MeetingSummary-Approved.pdf:p11pt1]\nLink: N/A\nFile: SC19-23_MeetingSummary-Approved.pdf\nLocation: page 11 part 1\nContent: Meeting Summary: 19th System Council Meeting 19th System Council Meeting SC19-23 20-21 October 2023, Rabat, Morocco Page 11 of 45 36. The Managing Director , Genetic Innovation , provided an overview of the current genetic innovation portfolio. This highlighted its consolidation into a unified program over the past three years, aiming to expedite genetic gain for climate change resilience, introduce new crop varieties, integrate gender -intentional and locally responsive market insights, and establish global breeding networks with partners. For the upcoming portfolio, plans include five unified Initiatives tailored to regional needs and market segments, wi th a specific emphasis on resource allocation for breeding and specialized asset funding mechanisms for genebanks. 37. The Resilient Agri-Food Systems (‘RAFS’) current portfolio was discussed, highlighting progress in impact orientation, partnerships, and systems thinking over the past three years. Two options for restructuring the next portfolio\n\n---\n\n[ID: pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p9pt1]\nLink: N/A\nFile: INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf\nLocation: page 9 part 1\nContent: CGIAR Initiative Proposal: Conservation and Use of Genetic Resources (Genebanks) 9 National genebanks : National genebank managers and government representatives collaborate and interact regularly with CGIAR genebanks, including at the Annual Genebanks Meeting organized by the CGIAR Genebank Platform; during the Initiative design process, national partners were involved in the Initiative Design Team. High-level stakeholders meetings: The Initiative design has been informed by stakeholder consultations with donors, national partners, private sector stakeholders, farmers’ groups and the Plant Treaty , including through the recent Genebank Costing and O perations (GCO) Review7 and subsequent Chatham House Dialogue5. These have influenced the content and structure of the Initiative. (Plant Treaty Letter of support) The Crop Trust: Consultations occurred with Crop Trust staff to discuss cooperation including specifically with BOLD and Seeds for Resilience projects targeted to national genebanks. (Crop Trust\n\n---\n\n[ID: pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p8pt4]\nLink: N/A\nFile: INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf\nLocation: page 8 part 4\nContent: pgr-genesys.org. Past data on germplasm distributions provides strong evidence for continued demand from both within and outside CGIAR from a wide range of users for the full range of crops being conserved by CGIAR genebanks from a wide for a range of purposes . Genebank users are surveyed to monitor their satisfaction with the service. A wide range of stakeholders and community members have been engaged in the design of the Genebanks Initiative, as follows. CGIAR Genebank managers: All CGIAR genebank managers have been regularly consulted and updated through meetings of the Article 15 group and the Platform Management Team, which has monthly meetings that include all genebank managers. These meetings were continued during the Initiative design process (with at least one per month since March 2021). CGIAR partners: Program-level planning meetings; during the I nitiative design process, discussions with other Initiatives were held, including those outside the GI Action\n\n---\n\n[ID: pdf:SC21-16_Meeting Summary_Approved.pdf:p46pt3]\nLink: N/A\nFile: SC21-16_Meeting Summary_Approved.pdf\nLocation: page 46 part 3\nContent: 2025 to feedback on the proposed governance and management of the Breeding for Tomorrow and Genebanks Science Program. d. Approval of the Integrated Partnership Risk &amp; Oversight Plan and endorsement of the IPB-AFRC and AOC implementation recommendations. e. Approval of the consolidated 2025–2027 workplan and budget for ISDC, SPIA, and IAES; noting ISDC’s review role and requesting Council approval if future asks exceed the budget uplift scenario. f. Request for Terms of Reference (by end -Q1 2025) for a 2025 review of CGIAR’s independent advisory functions, overseen by SIMEC with external experts. g. Request for a two-hour SPIA session in January 2025 for findings presentation and feedback. h. Approval of the 2025 Windows 1 &amp; 2 Budget, including financial plan, unrestricted funding allocations, and System activity financing approach. i. Request to form two working groups\n\n---\n\n[ID: pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p7pt1]\nLink: N/A\nFile: INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf\nLocation: page 7 part 1\nContent: CGIAR Initiative Proposal: Conservation and Use of Genetic Resources (Genebanks) 7 • provide facilitated access to PGRFA under their management in compliance with the conditions of the standard material transfer agreement; • recognize the authority of the Governing Body to provide policy guidance relating to ex situ collections held by them and subject to the provisions of the Treaty; and • manage and administer collections in accordance with internationally accepted standards, particularly the Genebank Standards endorsed by the FAO Commission on Genetic Resources for Food and Agriculture. Effective management and compliance with FAO standards and other relevant standards are achieved through implementing a quality management system based on optimized protocols for specific crops, facilities, locations, and situations. In collaboration with the Crop Trust, the Initiative will continue to update, audit, share and review at least 150 SOPs so that practices continue to comply with standards while being improved. Eight CGIAR genebanks are also committed to long-term agreements that obligate them to reach and sustain four performance\n\n---\n\n[ID: pdf:SC16-07_Meeting-Summary-APPROVED.pdf:p13pt2]\nLink: N/A\nFile: SC16-07_Meeting-Summary-APPROVED.pdf\nLocation: page 13 part 2\nContent: the impact sought from the 2022 -2024 interconnected portfolio is not delayed; and ii. Subject to anticipated developments in the political/regulatory landscape, revisit the funding arrangement in one year’s time and come back to the System Council with an ask for funding from the CGIAR Trust Fund at that time if considered appropriate. 26. The Global Director, Governance &amp; Assurance (a.i.) reaffirmed that CGIAR management is aligned with the System B oard’s position on not tabling the ‘Accelerating Crop Improvement Through Genome Editing ’ proposal for approval at this time, and its proposed approach of developing and providing to the System Council a memorandum on how the research can be taken forward in a timely way through appropriate funding arrangements. 27. The ISDC Chair affirmed that its review process, undertaken in accordance with that carried out for other CGIAR\n\n---\n\n[ID: pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p6pt4]\nLink: N/A\nFile: INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf\nLocation: page 6 part 4\nContent: Refinement of individual genebank budgets for essential operations. 2017–2021 Auditing of key standard operating procedures of genebanks Crop Trust • Compliance with FAO genebank standards, ISPM, SMTA, ASTI 2019–2020 Technical reviews of 11 Genebanks External reviewers • External validation of documented SOPS • Optimization of processes • Common data management system 2020 Chatham House consultation on future of genebanks Crop Trust &amp; CGIAR • Need for PGR in all future scenarios given increasing TUNA (turbulence, uncertainty, novelty, and ambiguousness). • CGIAR genebanks should play a more catalytic role to facilitate use of PGR. 2020 System Level Review of Genebank Costs and Operations CGIAR &amp; Crop Trust • Lock funding for essential operations • Review configuration of CGIAR genebanks • Underpinning roles of policy &amp; GHUs • Sustain CGIAR’s global system role\n\n---\n\n[ID: pdf:SC16-ChairSummary_July2022.pdf:p4pt2]\nLink: N/A\nFile: SC16-ChairSummary_July2022.pdf\nLocation: page 4 part 2\nContent: SC/M16/DP2: Adoption of the Agenda The System Council adopted the Agenda (document SC16-01). SC/M16/DP3: Evaluations Pursuant to Article 6.1 ff) of the CGIAR System Framework, the System Council endorsed the Evaluation of the CGIAR Platform for Excellence in Breeding and its accompanying management response. SC/M16/DP4: ISDC Membership &amp; Succession Pursuant to Articles 6.1 e) and f) of the CGIAR System Framework, the System Council: i. Appointed Professor Holger Meinke as Chair of CGIAR’s Independent Science for Development Council (‘ISDC’) for a second three -year term effective\n\n---\n\n[ID: pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p48pt2]\nLink: N/A\nFile: INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf\nLocation: page 48 part 2\nContent: genebank performance by Crop Trust Genebank performance targets: • % collection available for immediate distribution; • % collection safety duplicated; • Passport data completeness Index; • Minimum elements of quality management system. 2022, 2023, 2024 n/a • Influences allocation of endowment funding to management of individual collections; • Drives improvement in genebank performance. Other MELIA: Auditing and validation of SOPs Compliance with FAO, IPPC, SMTA genebank and germplasm exchange 2022, 2023, 2024 n/a • Recommendations lead to improved compliance; • In the event of continued lack of compliance additional actions\n\n---\n\n[ID: pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p49pt1]\nLink: N/A\nFile: INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf\nLocation: page 49 part 1\nContent: CGIAR Initiative Proposal: Conservation and Use of Genetic Resources (Genebanks) 49 7. Management plan and risk assessment 7.1 Management plan The Genebanks Initiative represents a long- term program of work that will benefit from a stable, system-level management structure. The Crop Trust will continue to provide specialist, independent oversight for the monitoring of genebank performance, which cove rs WP 1 . Overall Initiative management will be provided through the Genebank Program, where leaders of seed and clonal crops, Policy and GHU units will form\n\n---\n\n[ID: pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p49pt2]\nLink: N/A\nFile: INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf\nLocation: page 49 part 2\nContent: management will be provided through the Genebank Program, where leaders of seed and clonal crops, Policy and GHU units will form the Management Team under the Genebank Director. They will represent the genebank managers to support management decisions and priority re-setting in a similar way to the current Platform Management Team. Feedback from specific partners will influence the development and implementation of individual workplans (e.g., NPPOs, international policy fora, genebank community, etc). WPs 2 and 4 will be implemented by the same Communities of\n\n---\n\n[ID: pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p17pt4]\nLink: N/A\nFile: INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf\nLocation: page 17 part 4\nContent: the Genetic Innovation impact pathway. WP 1 directly feeds into and benefits from all the other WPs in the Genebanks Initiative and other CGIAR initiatives influencing all five Impact Areas, which provide improved intelligence technologies, policies, and tools to characterize or support the use of genetic resources, the pests and diseases that affect them, the trends in demand for them or the seed systems that adopt them. An important output of WP 1 is the satisfaction of users of genebank services. Time limits for requests to be addressed will be defined and monitored. Genebank operations are monitored by the Crop Trust as part of their oversight of long-term agreements funded by the endowment fund. The Crop Trust will audit at least 150 SOPs and organize five -yearly external reviews. Five seed collections are expected to reach performance targets and be eligible for increased endowment funding.\n\n---\n\n[ID: pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p55pt1]\nLink: N/A\nFile: INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf\nLocation: page 55 part 1\nContent: CGIAR Initiative Proposal: Conservation and Use of Genetic Resources (Genebanks) 55 8. Policy compliance, and oversight 8.1 Research governance Researchers involved in the implementation of this Initiative will comply with the procedures and policies determined by the System Board to be applicable to the delivery of research undertaken in furtherance of CGIAR’s 2030 Research and Innovation Strategy, thereby ensuring that all research meets applicable legal, regulatory and institutional requirements; appropriate ethical and scientific standards; and standards of quality, safety, privacy, ris k management and financial management . This includes CGIAR’s CGIAR Research Ethics Code and to the values, norms and behaviors in CG IAR’s Ethics Framework and in the Framework for Gender, Diversity and Inclusion in CGIAR’s\n\n---\n\n[ID: pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf:p12pt2]\nLink: N/A\nFile: INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS.pdf\nLocation: page 12 part 2\nContent: network.” “One of the aspects of this proposal that I think makes it stand apart from ot her proposals I have read is the ambition in scope of the Work Packages. With the five Work Packages, the proposal would modernize breeding program methods and structure, centralize resources for genotyping and analytics, improve safety and quality management, build [a] long-term data management system, and focus on innovation and change management. I think these changes are necessary to be able to reach the impact needs of the new One CGIAR organization as well as improving the many collaborating national programs.” “This [modernization] has been a challenge to implement at times but has allowed our breeding programs to continue to grow and to increase the rate of genetic gain and market share across crops. If we had not made these changes —including investments in IT, data management and systems, centralization of services, and predictive analytics, we would have struggled to continue to develop innovative solutions for our customers\n\n---\n\n[ID: pdf:INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf:p12pt2]\nLink: N/A\nFile: INIT04-Network-4-Enabling-Tools-Technologies-and-Shared-Services-N4ETTSS (1).pdf\nLocation: page 12 part 2\nContent: network.” “One of the aspects of this proposal that I think makes it stand apart from ot her proposals I have read is the ambition in scope of the Work Packages. With the five Work Packages, the proposal would modernize breeding program methods and structure, centralize resources for genotyping and analytics, improve safety and quality management, build [a] long-term data management system, and focus on innovation and change management. I think these changes are necessary to be able to reach the impact needs of the new One CGIAR organization as well as improving the many collaborating national programs.” “This [modernization] has been a challenge to implement at times but has allowed our breeding programs to continue to grow and to increase the rate of genetic gain and market share across crops. If we had not made these changes —including investments in IT, data management and systems, centralization of services, and predictive analytics, we would have struggled to continue to develop innovative solutions for our customers\n\n---\n\n[ID: pdf:SC20-19_Meeting Summary_APPROVED.pdf:p42pt4]\nLink: N/A\nFile: SC20-19_Meeting Summary_APPROVED.pdf\nLocation: page 42 part 4\nContent: the Strategic Impact, Monitoring and Evaluation Committee (SIMEC), provided a report on the SIMEC ’s activities, which included overseeing the functions of the advisory bodies, including the Independent Advisory and Evaluation Service (IAES), and the Standing Panel for Impact Assessment (SPIA). 118. Key points from the report included: a. Discussions on the SPIA budget, relating to the broader conversations about Window 1 budget allocation to core functions. b. Endorsement of the Genebank Platform Evaluation, being highly complementary of the Platform’s work in driving up standards across the system. c. Review of the evaluability assessment of the Regional Integrated Initiatives(RIIs), which highlighted issues such as lack of clear theory of change, limiting evaluation possibilities at the initiative level.\n\n---\n\n[ID: pdf:INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf:p49pt4]\nLink: N/A\nFile: INIT03-Conservation-and-Use-of-Genetic-Resources-Genebanks.pdf\nLocation: page 49 part 4\nContent: genebank users both within and external to CGIAR. Cross-initiative teams within the Genetic Innovation and other Action Areas, will be required to align efforts towards shared research goals. An Oversight Committee compri sing Initiative Management Team, CGIAR Board representatives, the Plant Treaty, and the Crop Trust will be formed to meet annually or more frequently to provide representation of the legal entities and major stakeholders in governance and strategic and risk management decisions. PGRFA policy representation and compliance decisions will be made by the\n\n---\n\n[ID: pdf:SC22-20_Meeting Summary_Approved.pdf:p13pt1]\nLink: N/A\nFile: SC22-20_Meeting Summary_Approved.pdf\nLocation: page 13 part 1\nContent: Meeting Summary: 22nd System Council Meeting 22nd CGIAR System Council Meeting SC22-20 4-5 June 2025, Penang, Malaysia Page 13 of 42 g. Genebanks: The importance of genebanks was raised, with appreciation for the unbundling of the genebanks from the Prog</t>
+  </si>
+  <si>
+    <t>[{"role": "system", "content": "You are a helpful assistant that answer user questions in a detailed and comprehensive way.\n\nAlways base your answer strictly on the provided context.\nProvide a detailed and comprehensive answer to the question.\nAfter the answer, add a section 'Used Sources:' followed by a comma-separated list of the IDs from the chunks you used in formulating the answer (e.g., pdf:doc1.pdf:p1pt1, docx:doc2.docx:u1-4). Only list chunks that directly contributed. Do not make up IDs."}, {"role": "user", "content": "Question: What were the System Council's decisions regarding appointments to the Intellectual Property Group?\n\nContext:\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row183]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 183\nContent: Decision: The System Council extended the membership of the following persons to the System Council Intellectual Property Group with effect until 31 December 2021, noting that such persons serve in a personal capacity and not as a representative of any of the System Council’s constituencies:\nDate(s): 24 March 2020\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row96]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 96\nContent: Decision: The System Council approved the formation and membership of an ad-hoc Nominations Committee, as follows: \ni) the Chair of the System Council’s Strategic Impact, Monitoring and Evaluation Committee (SIMEC), or their designate, acting as Chair of the Committee, \nii) the Chair of the System Council’s Assurance Oversight Committee (AOC), or their designate, and \niii) Alan Bennett acting as an independent member with expertise in intellectual property assets management;\nto select, for confirmation by the System Council, members of the System Council Intellectual Property Group ('SC IP Group') for a two-year term, in accordance with Section 3 of the SC IP Group’s Terms of Reference.\nDate(s): 23 March 2023\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row226]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 226\nContent: Decision: The System Council extends the membership of the following persons to the System Council Intellectual Property Group as an interim measure with effect until 31 December 2018, noting that such persons serve in a personal capacity and not as a representative of any of the System Council’s constituencies:\na. Paul Figueroa, Chair (Resident Legal Officer, USAID/Guatemala)\nb. Bram De Jonge, Member (Seed Policy Advisor OXFAM/Wageningen University)\nc. Aline Flower, Member (Associate General Counsel, Global Development, Bill and Melinda Gates Foundation)\nDate(s): 24 September 2018\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row208]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 208\nContent: Decision: The System Council extends the membership of the following persons to the System Council Intellectual Property Group with effect until 31 December 2019, noting that such persons serve in a personal capacity and not as a representative of any of the System Council’s constituencies: \n•Aline Flower, Member (Associate General Counsel, Global Development, Bill and Melinda Gates Foundation) nominated by Bill and Melinda Gates Foundation; and \n•Bram De Jonge, Member (Seed Policy Advisor OXFAM/Wageningen University) nominated by EIARD.\nDate(s): 13 March 2019\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row232]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 232\nContent: Decision: The System Council extends the membership of the following persons to the System Council Intellectual Property Group as an interim measure with effect until 31 July 2018, noting that such persons serve in a personal capacity and not as a representative of any of the System Council’s constituencies:\na. Paul Figueroa, Chair (Resident Legal Officer, USAID/Guatemala) nominated by USAID;\nb. Bram De Jonge, Member (Seed Policy Advisor OXFAM/Wageningen University) nominated by EIARD; and\nc. Aline Flower, Member (Associate General Counsel, Global Development, Bill and Melinda Gates Foundation) nominated by Bill and Melinda Gates Foundation.\nDate(s): 30 April 2018\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row94]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 94\nContent: Decision: Pursuant to paragraph 3 of Annex 1 to the CGIAR Intellectual Assets Principles, the System Council approved the Terms of Reference of the Ad-hoc Nominations Committee for membership of the System Council Intellectual Property Group.\nDate(s): 28 April 2023\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row85]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 85\nContent: Decision: The System Council approved the appointment of the following persons as members of the System Council Intellectual Property Group for a two-year term through 13 June 2025, noting that such persons serve in a personal capacity and not as a representative of any of the System Council’s constituencies:\n• Aline Flower (Associate General Counsel, Global Development, Bill &amp; Melinda Gates Foundation), nominated by the Bill &amp; Melinda Gates Foundation; and\n• Eric Huttner (Research Program Manager Crops, ACIAR), nominated by Australia.\nDate(s): 14 June 2023\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row1]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 1\nContent: Decision: Pursuant to the System Council Intellectual Property Group Terms of Reference, the System Council approved the appointment of the following persons as members of the System Council Intellectual Property Group for a two-year term, starting on 1 November 2025, noting that such persons serve in a personal capacity and not as a representative of any of the System Council’s constituencies: \n1.\tClément Aubert (Director of Innovation and Valorization ; Institut de Recherche pour le Développement), \n2.\tAline Flower (Deputy Director, Legal; Global Agricultural Development; Bill and Melinda Gates Foundation), and\n3.\tEric Huttner (Consultant, Chloroplast Consulting, as of September 2025, former Research Program Manager, Crops, Australian Centre for International Agricultural Research).\nDate(s): 14 October 2025\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row131]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 131\nContent: Decision: The System Council approved the extension of the following persons as members of the System Council Intellectual Property Group with effect until 31 October 2022, noting that such persons serve in a personal capacity and not as a representative of any of the System Council’s constituencies: \n\n•\tAline Flower, Member (Associate General Counsel, Global Development, Bill and Melinda Gates Foundation) originally nominated by Bill and Melinda Gates Foundation; and \n•\tBram De Jonge, Member (Seed Policy Advisor OXFAM/Wageningen University) originally nominated by EIARD.\nDate(s): 16 December 2021\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row265]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 265\nContent: Decision: The System Council ratifies as an interim measure with effect until 31 December 2017, the continuing membership of the System Council IP Group as follows, noting that such persons serve in a personal capacity and not as a representative of any of the System Council’s constituencies: \na. Paul Figueroa, Chair (Resident Legal Officer, USAID/Guatemala); \nb. Bram De Jonge, Member (Seed Policy Advisor OXFAM/Wageningen University); and \nc. Aline Flower, Member (Associate General Counsel, Global Development, Bill and Melinda Gates Foundation).\nDate(s): 17 February 2017\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row292]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 292\nContent: Decision: The System Council approved the Terms of Reference for the System Council Chair as set out in appendix 1 of meeting document SC1-02.\nDate(s): 12 July 2016\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row67]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 67\nContent: Decision: The System Council approved the Terms of Reference for the Nominations Committee of the System Council.\nDate(s): 20 March 2024\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row278]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 278\nContent: Decision: The System Council approved with immediate effect the rules of procedure for the System Council as set out in Appendix 1 to meeting document SC2-07.\nDate(s): 25 &amp; 26 September 2016\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row119]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 119\nContent: Decision: The System Council adopted the Agenda (document SC16-01).\nDate(s): 20 July 2022\n\n---\n\n[ID: pdf:SC22-14_AOC Report to SC22.pdf:p3pt3]\nLink: N/A\nFile: SC22-14_AOC Report to SC22.pdf\nLocation: page 3 part 3\nContent: items of the System Council’s Action Plan. To date, 11 of the 12 matters have been closed. For the remaining item on remuneration of governance officials, a review is being overseen by the Nominations Committee of the System Council, with results expected in mid-July 2025. The AOC notes that this will be a full year since the matter was first raised during SC20 in June 2024. 10. During the course of this work on the SC Action Plan, two further matters arose. One of these has been resolved and the other is in process. 11. The AOC submitted a report titled “System Council Action Plan and investigations: AOC conclusions and recommendations” to System Council V oting Members and Alternates on 21 March 2025, with an addendum on 14 April 2025. 12. The AOC provided an update on the System Council Action Plan to SC Voting Members and Alternates on 16 April 2025 and will provide a further update before the 22 nd System\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row293]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 293\nContent: Decision: The System Council adopted the meeting agenda for the 1st System Council meeting (document SC1-01).\nDate(s): 12 July 2016\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row281]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 281\nContent: Decision: The System Council adopted the Agenda as proposed in meeting document SC2-01.\nDate(s): 25 &amp; 26 September 2016\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row50]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 50\nContent: Decision: The System Council approved the Summary of the Ad Hoc Meeting of the System Council held on 24 July 2024\nDate(s): 22 August 2024\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row129]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 129\nContent: Decision: The System Council adopted the Agenda as issued on 7 March 2022 (document SC15-01, Revision 2).\nDate(s): 8-9 March 2022\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row49]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 49\nContent: Decision: The System Council appointed of Renaud Seligmann, representative of the World Bank to the System Council, as a member of the Assurance and Oversight Committee for a period of three years with effect from 12 September 2024, or until a successor is appointed.\nDate(s): 12 September 2024\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row78]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 78\nContent: Decision: The System Council adopted the Agenda, as re-issued on 18th October 2023 with revised timings and an additional item 13a titled ‘Reflections on Research Direction &amp; Funding’.\nDate(s): 21 October 2023\n\n---\n\n[ID: pdf:SC22-08 - Governance Updates.pdf:p3pt1]\nLink: N/A\nFile: SC22-08 - Governance Updates.pdf\nLocation: page 3 part 1\nContent: Framework and Charter Feedback documented for consideration in this next amendment process (summarized, non-exhaustive) 1 i. Roles of the System Council relating to IPB appointments ii. Refine roles/responsibilities relating to internal audit, external audit, ethics and risk management/internal controls to align with Risk &amp; Oversight Plan and address the AOC’s comments iii. Policy development\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row17]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 17\nContent: Decision: The System Council adopted the Agenda for the 22nd System Council meeting, as issued on 21 May 2025.\nDate(s): 4-5 June 2025\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row146]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 146\nContent: Decision: The System Council approved the extension of the terms of the following members of the System Council’s Assurance Oversight Committee until 30 June 2022, unless earlier determined by the System Council:\n• Saad Bounjoua\n• Maurice Goddard\n• Muriel Uzan\n• Daniel van Gilst\nDate(s): 10 June 2021\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row223]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 223\nContent: Decision: The System Council adopted the Agenda issued on 11 November 2018 (meeting document SC7-01).\nDate(s): 15-16 November 2018\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row143]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 143\nContent: Decision: The System Council approved the appointment of Dr. Raphael Nawrotzki, representative of Germany, on the System Council’s Strategic Impact, Monitoring and Evaluation Committee (SIMEC) for a period until 31 December 2021 or until such time as a successor is appointed.\nDate(s): 6 July 2021\n\n---\n\n[ID: pdf:SC22-20_Meeting Summary_Approved.pdf:p34pt3]\nLink: N/A\nFile: SC22-20_Meeting Summary_Approved.pdf\nLocation: page 34 part 3\nContent: an effective governance 113. The AOC Chair presented the Committee ’s key priorities for the remainder of 2025, which include overseeing ethics and business conduct matters, ensuring completion of the System Council Action Plan, providing input on upcoming Charter and Framework revisions, overseeing implementation of the ROP and related Council recommendations, advising on the Advisory Bodies’ business plans and budget, and supporting other Council activities as needed. 114. The AOC Chair presented two decision items for the Council, recognized the work of the Committee’s Secretary, and expressed gratitude to her fellow AOC members for their collaborative effort over the last months. Key Discussion Areas 115. Council members expressed their gratitude to the AOC for their work and dedication under short timelines. Specific points included: a. A suggestion that the terms of all System Council Committee Members be standardized to two, three-year terms, with exceptions for special\n\n---\n\n[ID: pdf:SC17-16_MeetingSummary_Approved_.pdf:p22pt4]\nLink: N/A\nFile: SC17-16_MeetingSummary_Approved_.pdf\nLocation: page 22 part 4\nContent: for Impa ct Assessment, the System Council confirm ed the appointments of the following persons: a. Dr. Kyle Emerick as SPIA Standing Panel Member for an additional three -year term with effect from 1 January 2023 unless otherwise decided by the System Council; and b. Dr. Rachid Laajaj as a Special Initiative Member for an additional three -year term with effect from 1 January 2023 unless otherwise decided by the System Council. 82. Decision SC/M17/DP6 - SIMEC Membership Appointments Pursuant to paragraph 9 of the terms of reference of the System Council’s Strategic Impact, Monitoring &amp; Evaluation Committee (‘SIMEC’), the System Council: a. Appointed the following persons as members of SIMEC until 30 June 2023 or such time as a successor is appointed:\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row205]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 205\nContent: Decision: The System Council adopted the Agenda issued on 23 April 2019 (meeting document SC8-01)\nDate(s): 15-16 May 2019\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row31]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 31\nContent: Decision: The System Council approved amendments to the Rules of Procedure of the System Council, in the form dated 27 November 2024, pursuant to paragraph 14.4 of those Rules of Procedure.\nDate(s): 11-12 December 2024\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row88]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 88\nContent: Decision: The System Council appointed Sebastian Lesch (Germany) as a second representative from the System Council on the Ad-Hoc Committee on Governance to provide continuity, noting that Andrew Campbell’s term on the System Council is anticipated to conclude at end-July 2023.\nDate(s): 12 May 2023\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row184]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 184\nContent: Decision: The System Council appointed Wijnand van-Ijssel (System Council member, The Netherlands) and Stephen Potter (System Council member, Canada) to serve in the role of System Council Active Observers on the System Management Board pursuant to Article 7.6 of the Charter of the System Organization effective from the date of this decision for a period of one year or until such time as a successor is appointed.\nDate(s): 24 March 2020\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row148]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 148\nContent: Decision: The System Council adopted the Agenda issued on 26 May 2021 (document SC13-01)\nDate(s): 9 June 2021\n\n---\n\n[ID: pdf:SC18-17_MeetingSummary_APPROVED.pdf:p2pt1]\nLink: N/A\nFile: SC18-17_MeetingSummary_APPROVED.pdf\nLocation: page 2 part 1\nContent: Meeting Summary, 18th System Council Meeting 18th System Council Meeting SC18-17 11-12 May 2023, Washington, DC, USA Page 2 of 42 Introduction This document presents a summary of the 18th meeting of the System Council (“Council”) held on 11-12 May 2023 in Washington, DC ., USA. It follows the release of the SC1 8 Chair’s Summary (25 May 2023). By way\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row162]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 162\nContent: Decision: The System Council approved the extension of the terms of the following membership on the System Council’s standing committees:\n- Stephen Potter (Canada), on the Assurance Oversight Committee to 30 June 2021, unless earlier determined by the System Council\n- The eight current members of the Strategic Impact, Monitoring and Evaluation Committee to 31 December 2021, unless earlier determined by the System Council\nDate(s): 17 December 2020\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row74]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 74\nContent: Decision: The System Council adopted the Agenda, as issued on 12 December 2023.\nDate(s): 20 December 2023\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row51]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 51\nContent: Decision: The System Council approved the \"Response from System Council to Management on the Risk and Oversight Action Plan (31 July 2024)\"\nDate(s): 14 August 2024\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row106]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 106\nContent: Decision: Pursuant to paragraph 9 of the terms of reference of the System Council’s Strategic Impact, Monitoring &amp; Evaluation Committee (‘SIMEC’), the System Council:\n\n(a)   Appoints the following persons as members of SIMEC until 30 June 2023 or such time as a successor is appointed\n\nNikita Eriksen-Hamel (Canada)\n\nGary Jahn (USA)\n\nFatma Sarsu (Türkiye)\n\n(b)  Retroactively extends the terms of all other members of SIMEC until 30 June 2023 or \n        such time as a successor is appointed.\nDate(s): 3 November 2022\n\n---\n\n[ID: pdf:SC22-Resource_SC-Action-Tracker.pdf:p1pt2]\nLink: N/A\nFile: SC22-Resource_SC-Action-Tracker.pdf\nLocation: page 1 part 2\nContent: additional resource for the System Council’s 22nd meeting sets out previously agreed action\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row189]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 189\nContent: Decision: The System Council adopted the Agenda issued on 8 November 2019 (document SC9-01).\nDate(s): 13-14 November 2019\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row60]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 60\nContent: Decision: The System Council adopted the Agenda for the 20th System Council meeting, as re-issued on 9 June 2024.\nDate(s): 13 June 2024\n\n---\n\n[ID: pdf:SC20_Chairs-Summary.pdf:p5pt1]\nLink: N/A\nFile: SC20_Chairs-Summary.pdf\nLocation: page 5 part 1\nContent: Chair’s Summary, SC20 20th CGIAR System Council Meeting Chair’s Summary, SC20 12-13 June 2024, Brasília, Brazil Page 5 of 5 AGREED POSITIONS AND ACTIONS SC20-AP1 – Requests to the Nominations Committee of the System Council The System Council requested the Nominations Committee of the System Council to: • Operate in accordance with its proposed, revised timeline for decision -making on Integrated Partnership Board (IPB) membership, including: o a revised delivery date of a slate of IPB nominees of Monday 22 July 2024; and o a proposal to convene a virtual, extraordinary System Council meeting session to decide on the slate of nominees, on Wednesday, 24 July 2024; and • Proceed with the selection of an external firm to be contracted by the System Organization in line with its procurement and contracting policies to review the\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row30]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 30\nContent: Decision: The System Council approved amendments to the Terms of Reference of the System Council Chair, in the form dated 27 November 2024, pursuant to Article 5.5 of the CGIAR System Framework.\nDate(s): 11-12 December 2024\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row251]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 251\nContent: Decision: The System Council adopted the Agenda, as issued on 18 October 2017.\nDate(s): 9-10 November 2017\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row230]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 230\nContent: Decision: The System Council adopted the Agenda issued on 2 May 2018 (meeting document SC6-01).\nDate(s): 16 May 2018\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row195]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 195\nContent: Decision: The System Council extended the membership term of Daniel van Gilst, System Council voting member, Norway, for the System Council’s Assurance Oversight Committee (‘AOC’) until 30 June 2021.\nDate(s): 15-16 May 2019\n\n---\n\n[ID: pdf:SC17-16_MeetingSummary_Approved_.pdf:p23pt1]\nLink: N/A\nFile: SC17-16_MeetingSummary_Approved_.pdf\nLocation: page 23 part 1\nContent: Meeting Summary: 17th System Council Meeting 17th System Council Meeting SC17-16 2-3 November 2022, Brisbane, Australia Page 23 of 32 i. Nikita Eriksen-Hamel (Canada) ii. Gary Jahn (USA) iii. Fatma Sarsu (Türkiye) b. Retroactively extends the terms of all other members of SIMEC until 30 June 2023 or such time as a successor is appointed. 83. Decision SC/M17/DP7 - AOC Membership Appointments Pursuant to paragraph 7 of the terms of reference of the System Council’s Assurance Oversight Committee, the System Council: a. Appointed Flora Mak (Canada) and Sarah Schmidt (Germany) as members of the Assurance Oversight Committee (‘AOC’) until 30 June 2023 or such time as their successors are appointed; and b. Retroactively extended the term of Muriel Uzán as a member of the AOC until 30 June 2023 or such time as a successor is appointed.\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row97]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 97\nContent: Decision: Pursuant to paragraph 7 of the terms of reference of the System Council’s Assurance Oversight Committee, the System Council appointed Fayezul Choudhury and Rita O’Sullivan as independent members of the Assurance Oversight Committee (‘AOC’) until 30 June 2023, or such time as their successors are appointed.\nDate(s): 15 February 2023\n\n---\n\n[ID: pdf:SC17-16_MeetingSummary_Approved_.pdf:p1pt2]\nLink: N/A\nFile: SC17-16_MeetingSummary_Approved_.pdf\nLocation: page 1 part 2\nContent: Council Meeting 2-3 November 2022 Purpose: This document presents the formal meeting summary for the System Council’s 1 7th meeting (‘SC17’), as approved by the System Council on a no\n\n---\n\n[ID: pdf:SC17-16_MeetingSummary_Approved_.pdf:p23pt2]\nLink: N/A\nFile: SC17-16_MeetingSummary_Approved_.pdf\nLocation: page 23 part 2\nContent: such time as their successors are appointed; and b. Retroactively extended the term of Muriel Uzán as a member of the AOC until 30 June 2023 or such time as a successor is appointed. Agenda Item 9: System Board and System Council responsibilities 84. In framing the session, t he session Chair indicated that, upon the System Board’s request, the System Council is being invited to reflect on a proposal to establish a small, joint cross -functional group to e xplore perceptions of inefficiencies and duplication across mandates, in a pragmatic and time-bound way. It was further noted that this was intended to be a discussion to consider incremental changes , versus fundamental transformation to the governing structure's architecture. 85. The Board Chair noted the Board’s awareness that there may be views of several System Council members\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row225]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 225\nContent: Decision: The System Council approved the document titled ‘Meeting Summary, 6th System Council meeting’ dated 1 October 2018\nDate(s): 30 October 2018\n\n---\n\n[ID: pdf:SC18-17_MeetingSummary_APPROVED.pdf:p10pt1]\nLink: N/A\nFile: SC18-17_MeetingSummary_APPROVED.pdf\nLocation: page 10 part 1\nContent: Meeting Summary: 18th System Council Meeting 18th System Council Meeting SC18-17 11-12 May 2023, Washington, DC, USA Page 10 of 42 (SPIA), pursuant to paragraph 6.6 of the SPIA terms of reference (TOR); b. Authorized SPIA to receive additional budget allocations through a flexible funding mechanism to supplement the pooled funding for the committed multi- year budgets; and c. Endorsed the revised SPIA TOR, pursuant to Articles 6.1 e) of the CGIAR System Framework. Agenda Item 5: Assurance and Oversight Committee (AOC) 26. At the invitation of the Co-Chair, the interim AOC Chair presented the AOC’s reflections and conclusions on the comprehensive review of the TOR, conducted in response to the Council’s request in November (SC17). 27. The presentation outlined the rationale for establishing the AOC as a standing committee of the Council and emphasized\n\n---\n\n[ID: pdf:SC22-Resource_SC-Action-Tracker.pdf:p1pt1]\nLink: N/A\nFile: SC22-Resource_SC-Action-Tracker.pdf\nLocation: page 1 part 1\nContent: Update on actions agreed with the System Council Purpose: This additional resource for\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row92]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 92\nContent: Decision: The System Council adopted the Agenda, as re-issued on 27 April 2023, with revised timings.\nDate(s): 12 May 2023\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row63]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 63\nContent: Decision: The System Council approved the Integrated Partnership Board Member Profile as presented by the Nominations Committee of the System Council.\nDate(s): 8 May 2024\n\n---\n\n[ID: pdf:SC22-14_AOC Report to SC22.pdf:p3pt2]\nLink: N/A\nFile: SC22-14_AOC Report to SC22.pdf\nLocation: page 3 part 2\nContent: opinion and the IPB -AFRC Chair is not aware of any qualified opinions received for any Center.1 7. The AOC appreciates the support of the IPB -AFRC and System Council in resolving the matters raised in the SC Action Plan and related investigations. The AOC has worked closely with the Office of Ethics and Business Conduct in overseeing various investigations and has benefited from the support of a non-conflicted consultant. 8. Ensuring that gaps in the CGIAR Charter and Framework – as raised by AOC – are effectively resolved will be an important workstream during the proposed Q3 revision sessions. AOC oversight of the System Council Action Plan and related matters 9. In 2025, the AOC continued its work to close the remaining items of the System Council’s Action Plan. To date, 11 of the 12 matters have been closed. For the remaining item on remuneration of governance officials, a review is being overseen by the Nominations Committee of the System Council, with\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row53]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 53\nContent: Decision: Consensus was reached to endorse the slate of Integrated Partnership Board members as recommended by the Nominations Committee of the System Council (five rolling over members and seven new members).\nDate(s): 24 July 2024\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row40]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 40\nContent: Decision: Pursuant to Article C. 7 of  AOC’s Terms of Reference, the System Council approves the establishment of an Ad Hoc Nominating Committee to identify and recommend for approval a candidate for the position of independent member of the Assurance and Oversight Committee that shall be made up of the current members of the AOC and a representative from the System Council\nDate(s): 1 November 2024\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row47]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 47\nContent: Decision: Pursuant to the authority as delegated to the System Council by the System Board under its role pursuant to Article 7.6 of the Charter of the CGIAR System Organization (System Board decision reference SB/M28/EDP1), the System Council:\n- Appointed the following persons to the Integrated Partnership Board for an initial term of three years from 1 October 2024 to 30 September 2027: Nicholas Austin; Ramesh Chand; Rachel Chikwamba; Jessica Fanzo; Segenet Kelemu; Mauricio Lopes; Celso Moretti; Dhesigen Naidoo; Enrica Porcari;\n- Reappointed the following persons to the Integrated Partnership Board for an additional term from 1 October 2024: Lindiwe Majele Sibanda (to 30 September 2027); Patrick Caron (to 30 September 2026); Alice Ruhweza (to 30 September 2026); Shenggen Fan (to 30 September 2026); Clarissa van Heerden (to 30 September 2026.\nDate(s): 27 September 2024\n\n---\n\n[ID: pdf:SC-adhoc-20December2023_MeetingSummary-APPROVED.pdf:p3pt2]\nLink: N/A\nFile: SC-adhoc-20December2023_MeetingSummary-APPROVED.pdf\nLocation: page 3 part 2\nContent: implementation. 8. In their interventions, System Council members were unanimous in their endorsement of the package of proposals in the Memorandum, and in their commendation of the Ad Hoc Committee on Governance for its stewardship of a constructive, collaborative and inclusive process to deliver an outcome and decision-making by the end of 2023. 9. Several System Council members called for additional detail to be provided around the intended role and responsibilities of the General Assembly of Centers, and its specific accountabilities in relation to the Integrated Partnership Board and the System Council. In particular, clarity was sought on its responsibilities relating to governance as well as being a forum for cross-Center interaction. (See action point SC19X-AP1) 10. Appreciation was expressed for the AOC’s\n\n---\n\n[ID: xlsx:CGIAR System Council Decisions.xlsx:row98]\nLink: N/A\nFile: CGIAR System Council Decisions.xlsx\nLocation: row 98\nContent: Decision: Pursuant to paragraph 9 of the terms of reference of the System Council’s Strategic Impact, Monitoring &amp; Evaluation Committee, the System Council appoints Dr. Didem Kökden as member of SIMEC until 30 June 2023</t>
   </si>
 </sst>
 </file>
@@ -5480,7 +5859,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5526,7 +5905,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C2">
         <v>200</v>
@@ -5538,22 +5917,22 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="H2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="J2" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="K2" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -5561,7 +5940,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C3">
         <v>200</v>
@@ -5573,22 +5952,22 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="I3" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="J3" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="K3" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -5596,7 +5975,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C4">
         <v>200</v>
@@ -5608,22 +5987,22 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H4" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="I4" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="J4" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="K4" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -5631,7 +6010,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C5">
         <v>200</v>
@@ -5643,22 +6022,22 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="I5" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="J5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="K5" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -5666,7 +6045,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C6">
         <v>200</v>
@@ -5678,22 +6057,22 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="I6" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="J6" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="K6" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -5701,7 +6080,7 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C7">
         <v>200</v>
@@ -5713,22 +6092,22 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="H7" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I7" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="J7" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="K7" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -5736,7 +6115,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C8">
         <v>200</v>
@@ -5748,22 +6127,22 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="H8" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="I8" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="J8" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="K8" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -5771,7 +6150,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C9">
         <v>200</v>
@@ -5783,22 +6162,22 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="I9" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="J9" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="K9" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -5806,7 +6185,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C10">
         <v>200</v>
@@ -5818,22 +6197,22 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G10" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="H10" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="I10" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="J10" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="K10" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -5841,7 +6220,7 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C11">
         <v>200</v>
@@ -5853,22 +6232,22 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H11" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="I11" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="J11" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="K11" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -5876,7 +6255,7 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C12">
         <v>200</v>
@@ -5888,22 +6267,22 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G12" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="H12" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="I12" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="J12" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="K12" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -5911,7 +6290,7 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C13">
         <v>200</v>
@@ -5923,22 +6302,22 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G13" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H13" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="I13" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="J13" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="K13" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -5946,7 +6325,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C14">
         <v>200</v>
@@ -5958,22 +6337,22 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G14" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="H14" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="I14" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="J14" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="K14" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -5981,7 +6360,7 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C15">
         <v>200</v>
@@ -5993,22 +6372,22 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G15" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="H15" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="I15" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="J15" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="K15" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -6016,7 +6395,7 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C16">
         <v>200</v>
@@ -6028,22 +6407,22 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G16" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H16" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="I16" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="J16" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="K16" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -6051,7 +6430,7 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C17">
         <v>200</v>
@@ -6063,22 +6442,22 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G17" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H17" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="I17" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="J17" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="K17" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -6086,7 +6465,7 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C18">
         <v>200</v>
@@ -6098,22 +6477,22 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G18" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H18" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="I18" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="J18" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="K18" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -6121,7 +6500,7 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C19">
         <v>200</v>
@@ -6133,22 +6512,22 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G19" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H19" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="I19" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="J19" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="K19" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -6156,7 +6535,7 @@
         <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C20">
         <v>200</v>
@@ -6168,22 +6547,22 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G20" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="H20" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="I20" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="J20" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="K20" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -6191,7 +6570,7 @@
         <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C21">
         <v>200</v>
@@ -6203,22 +6582,22 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G21" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H21" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="I21" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="J21" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="K21" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -6226,7 +6605,7 @@
         <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C22">
         <v>200</v>
@@ -6238,22 +6617,162 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G22" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H22" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="I22" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="J22" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="K22" t="s">
-        <v>121</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23">
+        <v>200</v>
+      </c>
+      <c r="D23">
+        <v>200</v>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" t="s">
+        <v>88</v>
+      </c>
+      <c r="I23" t="s">
+        <v>103</v>
+      </c>
+      <c r="J23" t="s">
+        <v>117</v>
+      </c>
+      <c r="K23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24">
+        <v>200</v>
+      </c>
+      <c r="D24">
+        <v>200</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" t="s">
+        <v>89</v>
+      </c>
+      <c r="I24" t="s">
+        <v>103</v>
+      </c>
+      <c r="J24" t="s">
+        <v>117</v>
+      </c>
+      <c r="K24" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25">
+        <v>200</v>
+      </c>
+      <c r="D25">
+        <v>200</v>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" t="s">
+        <v>64</v>
+      </c>
+      <c r="H25" t="s">
+        <v>90</v>
+      </c>
+      <c r="I25" t="s">
+        <v>103</v>
+      </c>
+      <c r="J25" t="s">
+        <v>117</v>
+      </c>
+      <c r="K25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26">
+        <v>200</v>
+      </c>
+      <c r="D26">
+        <v>200</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I26" t="s">
+        <v>103</v>
+      </c>
+      <c r="J26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K26" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>